<commit_message>
changed day name full to day name abbrev
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="cboc_signin_sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -422,6 +422,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
thick border for header
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -48,17 +48,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="00ff0000"/>
+      <left style="thick">
+        <color rgb="00001C54"/>
       </left>
-      <right style="double">
-        <color rgb="00ff0000"/>
+      <right style="thick">
+        <color rgb="00001C54"/>
       </right>
-      <top style="double">
-        <color rgb="00ff0000"/>
+      <top style="thick">
+        <color rgb="00001C54"/>
       </top>
-      <bottom style="double">
-        <color rgb="00ff0000"/>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
       </bottom>
     </border>
   </borders>

</xml_diff>

<commit_message>
b1 c1 border test
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -39,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -69,15 +69,24 @@
         <color rgb="00001C54"/>
       </bottom>
     </border>
+    <border>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -456,10 +465,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: March 2021</t>
+          <t>Month/Year: June 2021</t>
         </is>
       </c>
-      <c r="AE1" s="2" t="n"/>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="AE1" s="3" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
test of iter_rows loop
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -465,11 +465,38 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: June 2021</t>
+          <t>Month/Year: March 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
       <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="3" t="n"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test of adding cboc/core row
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,6 +30,11 @@
       <b val="1"/>
       <sz val="28"/>
     </font>
+    <font>
+      <name val="Times New Roman"/>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -39,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -77,17 +82,32 @@
         <color rgb="00001C54"/>
       </bottom>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -454,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +485,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: May 2021</t>
+          <t>Month/Year: June 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -499,6 +519,9 @@
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="3" t="n"/>
     </row>
+    <row r="2">
+      <c r="A2" s="4" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>

</xml_diff>

<commit_message>
corrected cboc/core col width
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -481,11 +481,14 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10.86" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: June 2021</t>
+          <t>Month/Year: April 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>

</xml_diff>

<commit_message>
re-ordered header to be after all other cells for easier formatting after merge
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -28,12 +28,12 @@
     <font>
       <name val="Times New Roman"/>
       <b val="1"/>
-      <sz val="28"/>
+      <sz val="10"/>
     </font>
     <font>
       <name val="Times New Roman"/>
       <b val="1"/>
-      <sz val="10"/>
+      <sz val="28"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,6 +56,20 @@
       <left style="thick">
         <color rgb="00001C54"/>
       </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
       <top style="thick">
         <color rgb="00001C54"/>
       </top>
@@ -75,20 +89,6 @@
       </bottom>
     </border>
     <border>
-      <top style="thick">
-        <color rgb="00001C54"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="00001C54"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="00001C54"/>
-      </left>
-      <right style="thick">
-        <color rgb="00001C54"/>
-      </right>
       <top style="thick">
         <color rgb="00001C54"/>
       </top>
@@ -102,12 +102,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>

</xml_diff>

<commit_message>
refactored header creating function
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -45,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -96,6 +96,50 @@
       <bottom style="thick">
         <color rgb="00001C54"/>
       </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -103,11 +147,11 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -489,7 +533,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: May 2021</t>
+          <t>Month/Year: April 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -541,14 +585,55 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Month/Year: April 2021</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AE1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added bash aliases to README.md
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -533,7 +533,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: April 2021</t>
+          <t>Month/Year: March 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -596,7 +596,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: April 2021</t>
+          <t>Month/Year: March 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>

</xml_diff>

<commit_message>
added .upper() to month name in header
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="1-15" sheetId="1" state="visible" r:id="rId1"/>
@@ -143,21 +143,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -515,7 +515,6 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <tabColor rgb="001072BA"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -527,13 +526,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.86" customWidth="1" min="1" max="1"/>
+    <col customWidth="1" max="1" min="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: March 2021</t>
+          <t>Month/Year: DECEMBER 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -574,14 +573,13 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <tabColor rgb="001072BA"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -596,7 +594,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: March 2021</t>
+          <t>Month/Year: DECEMBER 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -634,6 +632,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify user input to mm/yy format
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -532,7 +532,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: DECEMBER 2021</t>
+          <t>Month/Year: APRIL 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -594,7 +594,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: DECEMBER 2021</t>
+          <t>Month/Year: APRIL 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>

</xml_diff>

<commit_message>
changed user input to mm/yy format and refactored get start date function
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -532,7 +532,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: APRIL 2021</t>
+          <t>Month/Year: MARCH 2024</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -594,7 +594,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: APRIL 2021</t>
+          <t>Month/Year: MARCH 2024</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>

</xml_diff>

<commit_message>
added input validation to user input
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-15" sheetId="1" state="visible" r:id="rId1"/>
@@ -143,21 +143,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -526,13 +526,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="10.86"/>
+    <col width="10.86" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MARCH 2024</t>
+          <t>Month/Year: DECEMBER 2022</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -573,7 +573,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -594,7 +594,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MARCH 2024</t>
+          <t>Month/Year: DECEMBER 2022</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -632,6 +632,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added int() comparison for year strings
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -532,7 +532,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: DECEMBER 2022</t>
+          <t>Month/Year: MARCH 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -594,7 +594,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: DECEMBER 2022</t>
+          <t>Month/Year: MARCH 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>

</xml_diff>

<commit_message>
fixed num digit check for user input
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="1-15" sheetId="1" state="visible" r:id="rId1"/>
@@ -143,21 +143,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -526,13 +526,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.86" customWidth="1" min="1" max="1"/>
+    <col customWidth="1" max="1" min="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MARCH 2021</t>
+          <t>Month/Year: FEBRUARY 2023</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -573,7 +573,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -594,7 +594,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MARCH 2021</t>
+          <t>Month/Year: FEBRUARY 2023</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -632,6 +632,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added end date calculation
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -532,7 +532,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2023</t>
+          <t>Month/Year: FEBRUARY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -594,7 +594,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2023</t>
+          <t>Month/Year: FEBRUARY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>

</xml_diff>

<commit_message>
start of using rows/cols for accessing cells instead of letters. ready to create cboc cell font/border/value function
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -567,7 +567,11 @@
       <c r="AE1" s="3" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n"/>
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
test setting header row height
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-15" sheetId="1" state="visible" r:id="rId1"/>
@@ -143,21 +143,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -526,13 +526,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="10.86"/>
+    <col width="10.86" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2021</t>
+          <t>Month/Year: APRIL 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -577,7 +577,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -598,7 +598,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2021</t>
+          <t>Month/Year: APRIL 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -636,6 +636,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed set row height (had accidentally set row width)
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -529,7 +529,7 @@
     <col width="10.86" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Month/Year: APRIL 2021</t>
@@ -595,7 +595,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Month/Year: APRIL 2021</t>

</xml_diff>

<commit_message>
modified all row height for both sheets
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -566,13 +566,37 @@
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="3" t="n"/>
     </row>
-    <row r="2">
+    <row r="2" ht="20" customHeight="1">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
     </row>
+    <row r="3" ht="22" customHeight="1"/>
+    <row r="4" ht="27" customHeight="1"/>
+    <row r="5" ht="21" customHeight="1"/>
+    <row r="6" ht="21" customHeight="1"/>
+    <row r="7" ht="10" customHeight="1"/>
+    <row r="8" ht="21" customHeight="1"/>
+    <row r="9" ht="21" customHeight="1"/>
+    <row r="10" ht="10" customHeight="1"/>
+    <row r="11" ht="21" customHeight="1"/>
+    <row r="12" ht="21" customHeight="1"/>
+    <row r="13" ht="10" customHeight="1"/>
+    <row r="14" ht="21" customHeight="1"/>
+    <row r="15" ht="10" customHeight="1"/>
+    <row r="16" ht="10" customHeight="1"/>
+    <row r="17" ht="21" customHeight="1"/>
+    <row r="18" ht="21" customHeight="1"/>
+    <row r="19" ht="10" customHeight="1"/>
+    <row r="20" ht="21" customHeight="1"/>
+    <row r="21" ht="21" customHeight="1"/>
+    <row r="22" ht="10" customHeight="1"/>
+    <row r="23" ht="21" customHeight="1"/>
+    <row r="24" ht="21" customHeight="1"/>
+    <row r="26" ht="21" customHeight="1"/>
+    <row r="27" ht="21" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
@@ -632,6 +656,31 @@
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="3" t="n"/>
     </row>
+    <row r="2" ht="20" customHeight="1"/>
+    <row r="3" ht="22" customHeight="1"/>
+    <row r="4" ht="27" customHeight="1"/>
+    <row r="5" ht="21" customHeight="1"/>
+    <row r="6" ht="21" customHeight="1"/>
+    <row r="7" ht="10" customHeight="1"/>
+    <row r="8" ht="21" customHeight="1"/>
+    <row r="9" ht="21" customHeight="1"/>
+    <row r="10" ht="10" customHeight="1"/>
+    <row r="11" ht="21" customHeight="1"/>
+    <row r="12" ht="21" customHeight="1"/>
+    <row r="13" ht="10" customHeight="1"/>
+    <row r="14" ht="21" customHeight="1"/>
+    <row r="15" ht="10" customHeight="1"/>
+    <row r="16" ht="10" customHeight="1"/>
+    <row r="17" ht="21" customHeight="1"/>
+    <row r="18" ht="21" customHeight="1"/>
+    <row r="19" ht="10" customHeight="1"/>
+    <row r="20" ht="21" customHeight="1"/>
+    <row r="21" ht="21" customHeight="1"/>
+    <row r="22" ht="10" customHeight="1"/>
+    <row r="23" ht="21" customHeight="1"/>
+    <row r="24" ht="21" customHeight="1"/>
+    <row r="26" ht="21" customHeight="1"/>
+    <row r="27" ht="21" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>

</xml_diff>

<commit_message>
using actual dates for second sheet
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -18,18 +18,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <b val="1"/>
-      <sz val="10"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -57,6 +52,14 @@
       <left style="thick">
         <color rgb="00001C54"/>
       </left>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thick">
         <color rgb="00001C54"/>
       </right>
@@ -68,28 +71,20 @@
       </bottom>
     </border>
     <border>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thick">
         <color rgb="00001C54"/>
       </left>
-      <top style="thick">
-        <color rgb="00001C54"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="00001C54"/>
-      </bottom>
-    </border>
-    <border>
       <right style="thick">
         <color rgb="00001C54"/>
       </right>
-      <top style="thick">
-        <color rgb="00001C54"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="00001C54"/>
-      </bottom>
-    </border>
-    <border>
       <top style="thick">
         <color rgb="00001C54"/>
       </top>
@@ -145,14 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -518,7 +512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,113 +542,7 @@
       <c r="L1" s="2" t="n"/>
       <c r="M1" s="2" t="n"/>
       <c r="N1" s="2" t="n"/>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="2" t="n"/>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="2" t="n"/>
-      <c r="T1" s="2" t="n"/>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="2" t="n"/>
-      <c r="W1" s="2" t="n"/>
-      <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="2" t="n"/>
-      <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-      <c r="AE1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="22" customHeight="1"/>
-    <row r="4" ht="27" customHeight="1"/>
-    <row r="5" ht="21" customHeight="1"/>
-    <row r="6" ht="21" customHeight="1"/>
-    <row r="7" ht="10" customHeight="1"/>
-    <row r="8" ht="21" customHeight="1"/>
-    <row r="9" ht="21" customHeight="1"/>
-    <row r="10" ht="10" customHeight="1"/>
-    <row r="11" ht="21" customHeight="1"/>
-    <row r="12" ht="21" customHeight="1"/>
-    <row r="13" ht="10" customHeight="1"/>
-    <row r="14" ht="21" customHeight="1"/>
-    <row r="15" ht="10" customHeight="1"/>
-    <row r="16" ht="10" customHeight="1"/>
-    <row r="17" ht="21" customHeight="1"/>
-    <row r="18" ht="21" customHeight="1"/>
-    <row r="19" ht="10" customHeight="1"/>
-    <row r="20" ht="21" customHeight="1"/>
-    <row r="21" ht="21" customHeight="1"/>
-    <row r="22" ht="10" customHeight="1"/>
-    <row r="23" ht="21" customHeight="1"/>
-    <row r="24" ht="21" customHeight="1"/>
-    <row r="26" ht="21" customHeight="1"/>
-    <row r="27" ht="21" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:AE1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AE1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" ht="45" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Month/Year: APRIL 2021</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-      <c r="K1" s="2" t="n"/>
-      <c r="L1" s="2" t="n"/>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="2" t="n"/>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="2" t="n"/>
-      <c r="T1" s="2" t="n"/>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="2" t="n"/>
-      <c r="W1" s="2" t="n"/>
-      <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="2" t="n"/>
-      <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-      <c r="AE1" s="3" t="n"/>
+      <c r="O1" s="3" t="n"/>
     </row>
     <row r="2" ht="20" customHeight="1"/>
     <row r="3" ht="22" customHeight="1"/>
@@ -683,7 +571,75 @@
     <row r="27" ht="21" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" ht="45" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Month/Year: APRIL 2021</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="20" customHeight="1"/>
+    <row r="3" ht="22" customHeight="1"/>
+    <row r="4" ht="27" customHeight="1"/>
+    <row r="5" ht="21" customHeight="1"/>
+    <row r="6" ht="21" customHeight="1"/>
+    <row r="7" ht="10" customHeight="1"/>
+    <row r="8" ht="21" customHeight="1"/>
+    <row r="9" ht="21" customHeight="1"/>
+    <row r="10" ht="10" customHeight="1"/>
+    <row r="11" ht="21" customHeight="1"/>
+    <row r="12" ht="21" customHeight="1"/>
+    <row r="13" ht="10" customHeight="1"/>
+    <row r="14" ht="21" customHeight="1"/>
+    <row r="15" ht="10" customHeight="1"/>
+    <row r="16" ht="10" customHeight="1"/>
+    <row r="17" ht="21" customHeight="1"/>
+    <row r="18" ht="21" customHeight="1"/>
+    <row r="19" ht="10" customHeight="1"/>
+    <row r="20" ht="21" customHeight="1"/>
+    <row r="21" ht="21" customHeight="1"/>
+    <row r="22" ht="10" customHeight="1"/>
+    <row r="23" ht="21" customHeight="1"/>
+    <row r="24" ht="21" customHeight="1"/>
+    <row r="26" ht="21" customHeight="1"/>
+    <row r="27" ht="21" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
testing a month w 13 days in second sheet
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -526,7 +526,7 @@
     <row r="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: APRIL 2021</t>
+          <t>Month/Year: FEBRUARY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -583,7 +583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,7 +594,7 @@
     <row r="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: APRIL 2021</t>
+          <t>Month/Year: FEBRUARY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -608,9 +608,7 @@
       <c r="J1" s="2" t="n"/>
       <c r="K1" s="2" t="n"/>
       <c r="L1" s="2" t="n"/>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
-      <c r="O1" s="3" t="n"/>
+      <c r="M1" s="3" t="n"/>
     </row>
     <row r="2" ht="20" customHeight="1"/>
     <row r="3" ht="22" customHeight="1"/>
@@ -639,7 +637,7 @@
     <row r="27" ht="21" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed date * 2 + 1 for header to be num of cols
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -512,7 +512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
     <row r="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2021</t>
+          <t>Month/Year: APRIL 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -542,7 +542,23 @@
       <c r="L1" s="2" t="n"/>
       <c r="M1" s="2" t="n"/>
       <c r="N1" s="2" t="n"/>
-      <c r="O1" s="3" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="3" t="n"/>
     </row>
     <row r="2" ht="20" customHeight="1"/>
     <row r="3" ht="22" customHeight="1"/>
@@ -571,7 +587,7 @@
     <row r="27" ht="21" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:AE1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -583,7 +599,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,7 +610,7 @@
     <row r="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2021</t>
+          <t>Month/Year: APRIL 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -608,7 +624,25 @@
       <c r="J1" s="2" t="n"/>
       <c r="K1" s="2" t="n"/>
       <c r="L1" s="2" t="n"/>
-      <c r="M1" s="3" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="3" t="n"/>
     </row>
     <row r="2" ht="20" customHeight="1"/>
     <row r="3" ht="22" customHeight="1"/>
@@ -637,7 +671,7 @@
     <row r="27" ht="21" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:AE1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
with cboc column working!
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="1-15" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,13 +18,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <b val="1"/>
+      <sz val="9"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -40,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -52,6 +57,9 @@
       <left style="thick">
         <color rgb="00001C54"/>
       </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
       <top style="thick">
         <color rgb="00001C54"/>
       </top>
@@ -60,6 +68,61 @@
       </bottom>
     </border>
     <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <top style="thick">
+        <color rgb="00001C54"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thick">
         <color rgb="00001C54"/>
       </right>
@@ -71,20 +134,6 @@
       </bottom>
     </border>
     <border>
-      <top style="thick">
-        <color rgb="00001C54"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="00001C54"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="00001C54"/>
-      </left>
-      <right style="thick">
-        <color rgb="00001C54"/>
-      </right>
       <top style="thick">
         <color rgb="00001C54"/>
       </top>
@@ -138,20 +187,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="9">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -512,7 +566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,13 +574,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.86" customWidth="1" min="1" max="1"/>
+    <col customWidth="1" max="1" min="1" width="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: APRIL 2021</t>
+          <t>Month/Year: MAY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -560,36 +614,161 @@
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="3" t="n"/>
     </row>
-    <row r="2" ht="20" customHeight="1"/>
-    <row r="3" ht="22" customHeight="1"/>
-    <row r="4" ht="27" customHeight="1"/>
-    <row r="5" ht="21" customHeight="1"/>
-    <row r="6" ht="21" customHeight="1"/>
-    <row r="7" ht="10" customHeight="1"/>
-    <row r="8" ht="21" customHeight="1"/>
-    <row r="9" ht="21" customHeight="1"/>
-    <row r="10" ht="10" customHeight="1"/>
-    <row r="11" ht="21" customHeight="1"/>
-    <row r="12" ht="21" customHeight="1"/>
-    <row r="13" ht="10" customHeight="1"/>
-    <row r="14" ht="21" customHeight="1"/>
-    <row r="15" ht="10" customHeight="1"/>
-    <row r="16" ht="10" customHeight="1"/>
-    <row r="17" ht="21" customHeight="1"/>
-    <row r="18" ht="21" customHeight="1"/>
-    <row r="19" ht="10" customHeight="1"/>
-    <row r="20" ht="21" customHeight="1"/>
-    <row r="21" ht="21" customHeight="1"/>
-    <row r="22" ht="10" customHeight="1"/>
-    <row r="23" ht="21" customHeight="1"/>
-    <row r="24" ht="21" customHeight="1"/>
-    <row r="26" ht="21" customHeight="1"/>
-    <row r="27" ht="21" customHeight="1"/>
+    <row customHeight="1" ht="20" r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>CBOC/CORE</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="22" r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="27" r="4">
+      <c r="A4" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>Oak Lawn</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="7">
+      <c r="A7" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>Hoffman Est.</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="10">
+      <c r="A10" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>Aurora</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="12">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="13">
+      <c r="A13" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>Kankakee</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="16">
+      <c r="A16" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>LaSalle</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="18">
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="19">
+      <c r="A19" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>Joliet</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="22">
+      <c r="A22" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>Jesse Brown</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="24">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="25">
+      <c r="A25" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>Crown Point</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -599,18 +778,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AG27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="11"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: APRIL 2021</t>
+          <t>Month/Year: MAY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -642,37 +824,164 @@
       <c r="AB1" s="2" t="n"/>
       <c r="AC1" s="2" t="n"/>
       <c r="AD1" s="2" t="n"/>
-      <c r="AE1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="20" customHeight="1"/>
-    <row r="3" ht="22" customHeight="1"/>
-    <row r="4" ht="27" customHeight="1"/>
-    <row r="5" ht="21" customHeight="1"/>
-    <row r="6" ht="21" customHeight="1"/>
-    <row r="7" ht="10" customHeight="1"/>
-    <row r="8" ht="21" customHeight="1"/>
-    <row r="9" ht="21" customHeight="1"/>
-    <row r="10" ht="10" customHeight="1"/>
-    <row r="11" ht="21" customHeight="1"/>
-    <row r="12" ht="21" customHeight="1"/>
-    <row r="13" ht="10" customHeight="1"/>
-    <row r="14" ht="21" customHeight="1"/>
-    <row r="15" ht="10" customHeight="1"/>
-    <row r="16" ht="10" customHeight="1"/>
-    <row r="17" ht="21" customHeight="1"/>
-    <row r="18" ht="21" customHeight="1"/>
-    <row r="19" ht="10" customHeight="1"/>
-    <row r="20" ht="21" customHeight="1"/>
-    <row r="21" ht="21" customHeight="1"/>
-    <row r="22" ht="10" customHeight="1"/>
-    <row r="23" ht="21" customHeight="1"/>
-    <row r="24" ht="21" customHeight="1"/>
-    <row r="26" ht="21" customHeight="1"/>
-    <row r="27" ht="21" customHeight="1"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="20" r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>CBOC/CORE</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="22" r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="27" r="4">
+      <c r="A4" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>Oak Lawn</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="7">
+      <c r="A7" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>Hoffman Est.</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="10">
+      <c r="A10" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>Aurora</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="12">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="13">
+      <c r="A13" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>Kankakee</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="16">
+      <c r="A16" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>LaSalle</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="18">
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="19">
+      <c r="A19" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>Joliet</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="22">
+      <c r="A22" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>Jesse Brown</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="24">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="10" r="25">
+      <c r="A25" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="21" r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>Crown Point</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="21" r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>Frozen</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A1:AG1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test w new cboc col
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -574,13 +574,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="11"/>
+    <col customWidth="1" max="1" min="1" width="11.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: JUNE 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -778,7 +778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,13 +786,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="11"/>
+    <col customWidth="1" max="1" min="1" width="11.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: JUNE 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -824,9 +824,7 @@
       <c r="AB1" s="2" t="n"/>
       <c r="AC1" s="2" t="n"/>
       <c r="AD1" s="2" t="n"/>
-      <c r="AE1" s="2" t="n"/>
-      <c r="AF1" s="2" t="n"/>
-      <c r="AG1" s="3" t="n"/>
+      <c r="AE1" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
@@ -980,7 +978,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="A1:AE1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed column_dimensions.width so it can use the column number instead of letter
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="1-15" sheetId="1" state="visible" r:id="rId1"/>
@@ -187,25 +187,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -574,10 +574,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.5" customWidth="1" min="1" max="1"/>
+    <col customWidth="1" max="1" min="1" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Month/Year: MAY 2021</t>
@@ -614,150 +614,150 @@
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="3" t="n"/>
     </row>
-    <row r="2" ht="20" customHeight="1">
+    <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>CBOC/CORE</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="22" customHeight="1">
+    <row customHeight="1" ht="22" r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="27" customHeight="1">
+    <row customHeight="1" ht="27" r="4">
       <c r="A4" s="6" t="n"/>
     </row>
-    <row r="5" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="6">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="7">
       <c r="A7" s="6" t="n"/>
     </row>
-    <row r="8" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="8">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="10">
       <c r="A10" s="6" t="n"/>
     </row>
-    <row r="11" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="11">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="12">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="13">
       <c r="A13" s="6" t="n"/>
     </row>
-    <row r="14" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="14">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="15">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="16">
       <c r="A16" s="6" t="n"/>
     </row>
-    <row r="17" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="17">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="19" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="19">
       <c r="A19" s="6" t="n"/>
     </row>
-    <row r="20" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="20">
       <c r="A20" s="7" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="22">
       <c r="A22" s="6" t="n"/>
     </row>
-    <row r="23" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="23">
       <c r="A23" s="7" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="24">
       <c r="A24" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="25">
       <c r="A25" s="6" t="n"/>
     </row>
-    <row r="26" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="26">
       <c r="A26" s="7" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Frozen</t>
@@ -768,7 +768,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -786,10 +786,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.5" customWidth="1" min="1" max="1"/>
+    <col customWidth="1" max="1" min="1" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Month/Year: MAY 2021</t>
@@ -828,150 +828,150 @@
       <c r="AF1" s="2" t="n"/>
       <c r="AG1" s="3" t="n"/>
     </row>
-    <row r="2" ht="20" customHeight="1">
+    <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>CBOC/CORE</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="22" customHeight="1">
+    <row customHeight="1" ht="22" r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="27" customHeight="1">
+    <row customHeight="1" ht="27" r="4">
       <c r="A4" s="6" t="n"/>
     </row>
-    <row r="5" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="6">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="7">
       <c r="A7" s="6" t="n"/>
     </row>
-    <row r="8" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="8">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="10">
       <c r="A10" s="6" t="n"/>
     </row>
-    <row r="11" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="11">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="12">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="13">
       <c r="A13" s="6" t="n"/>
     </row>
-    <row r="14" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="14">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="15">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="16">
       <c r="A16" s="6" t="n"/>
     </row>
-    <row r="17" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="17">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="19" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="19">
       <c r="A19" s="6" t="n"/>
     </row>
-    <row r="20" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="20">
       <c r="A20" s="7" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="22">
       <c r="A22" s="6" t="n"/>
     </row>
-    <row r="23" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="23">
       <c r="A23" s="7" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="24">
       <c r="A24" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="25">
       <c r="A25" s="6" t="n"/>
     </row>
-    <row r="26" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="26">
       <c r="A26" s="7" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Frozen</t>
@@ -982,6 +982,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AG1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
start of create date cols
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -580,7 +580,7 @@
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: FEBRUARY 2024</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -778,7 +778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AC27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -792,7 +792,7 @@
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: FEBRUARY 2024</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -822,11 +822,7 @@
       <c r="Z1" s="2" t="n"/>
       <c r="AA1" s="2" t="n"/>
       <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-      <c r="AE1" s="2" t="n"/>
-      <c r="AF1" s="2" t="n"/>
-      <c r="AG1" s="3" t="n"/>
+      <c r="AC1" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
@@ -980,7 +976,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="A1:AC1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed end col for create date cols function
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -580,7 +580,7 @@
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2024</t>
+          <t>Month/Year: MAY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -778,7 +778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC27"/>
+  <dimension ref="A1:AG27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -792,7 +792,7 @@
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2024</t>
+          <t>Month/Year: MAY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -822,7 +822,11 @@
       <c r="Z1" s="2" t="n"/>
       <c r="AA1" s="2" t="n"/>
       <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="3" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
@@ -976,7 +980,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="A1:AG1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
making reg date row cols same width
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -575,6 +575,36 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="11.5"/>
+    <col customWidth="1" max="2" min="2" width="4.5"/>
+    <col customWidth="1" max="3" min="3" width="4.5"/>
+    <col customWidth="1" max="4" min="4" width="4.5"/>
+    <col customWidth="1" max="5" min="5" width="4.5"/>
+    <col customWidth="1" max="6" min="6" width="4.5"/>
+    <col customWidth="1" max="7" min="7" width="4.5"/>
+    <col customWidth="1" max="8" min="8" width="4.5"/>
+    <col customWidth="1" max="9" min="9" width="4.5"/>
+    <col customWidth="1" max="10" min="10" width="4.5"/>
+    <col customWidth="1" max="11" min="11" width="4.5"/>
+    <col customWidth="1" max="12" min="12" width="4.5"/>
+    <col customWidth="1" max="13" min="13" width="4.5"/>
+    <col customWidth="1" max="14" min="14" width="4.5"/>
+    <col customWidth="1" max="15" min="15" width="4.5"/>
+    <col customWidth="1" max="16" min="16" width="4.5"/>
+    <col customWidth="1" max="17" min="17" width="4.5"/>
+    <col customWidth="1" max="18" min="18" width="4.5"/>
+    <col customWidth="1" max="19" min="19" width="4.5"/>
+    <col customWidth="1" max="20" min="20" width="4.5"/>
+    <col customWidth="1" max="21" min="21" width="4.5"/>
+    <col customWidth="1" max="22" min="22" width="4.5"/>
+    <col customWidth="1" max="23" min="23" width="4.5"/>
+    <col customWidth="1" max="24" min="24" width="4.5"/>
+    <col customWidth="1" max="25" min="25" width="4.5"/>
+    <col customWidth="1" max="26" min="26" width="4.5"/>
+    <col customWidth="1" max="27" min="27" width="4.5"/>
+    <col customWidth="1" max="28" min="28" width="4.5"/>
+    <col customWidth="1" max="29" min="29" width="4.5"/>
+    <col customWidth="1" max="30" min="30" width="4.5"/>
+    <col customWidth="1" max="31" min="31" width="4.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45" r="1">
@@ -787,6 +817,38 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="11.5"/>
+    <col customWidth="1" max="2" min="2" width="4.5"/>
+    <col customWidth="1" max="3" min="3" width="4.5"/>
+    <col customWidth="1" max="4" min="4" width="4.5"/>
+    <col customWidth="1" max="5" min="5" width="4.5"/>
+    <col customWidth="1" max="6" min="6" width="4.5"/>
+    <col customWidth="1" max="7" min="7" width="4.5"/>
+    <col customWidth="1" max="8" min="8" width="4.5"/>
+    <col customWidth="1" max="9" min="9" width="4.5"/>
+    <col customWidth="1" max="10" min="10" width="4.5"/>
+    <col customWidth="1" max="11" min="11" width="4.5"/>
+    <col customWidth="1" max="12" min="12" width="4.5"/>
+    <col customWidth="1" max="13" min="13" width="4.5"/>
+    <col customWidth="1" max="14" min="14" width="4.5"/>
+    <col customWidth="1" max="15" min="15" width="4.5"/>
+    <col customWidth="1" max="16" min="16" width="4.5"/>
+    <col customWidth="1" max="17" min="17" width="4.5"/>
+    <col customWidth="1" max="18" min="18" width="4.5"/>
+    <col customWidth="1" max="19" min="19" width="4.5"/>
+    <col customWidth="1" max="20" min="20" width="4.5"/>
+    <col customWidth="1" max="21" min="21" width="4.5"/>
+    <col customWidth="1" max="22" min="22" width="4.5"/>
+    <col customWidth="1" max="23" min="23" width="4.5"/>
+    <col customWidth="1" max="24" min="24" width="4.5"/>
+    <col customWidth="1" max="25" min="25" width="4.5"/>
+    <col customWidth="1" max="26" min="26" width="4.5"/>
+    <col customWidth="1" max="27" min="27" width="4.5"/>
+    <col customWidth="1" max="28" min="28" width="4.5"/>
+    <col customWidth="1" max="29" min="29" width="4.5"/>
+    <col customWidth="1" max="30" min="30" width="4.5"/>
+    <col customWidth="1" max="31" min="31" width="4.5"/>
+    <col customWidth="1" max="32" min="32" width="4.5"/>
+    <col customWidth="1" max="33" min="33" width="4.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45" r="1">

</xml_diff>

<commit_message>
have set for upper case day name
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-15" sheetId="1" state="visible" r:id="rId1"/>
@@ -187,25 +187,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -574,43 +574,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="11.5"/>
-    <col customWidth="1" max="2" min="2" width="4.5"/>
-    <col customWidth="1" max="3" min="3" width="4.5"/>
-    <col customWidth="1" max="4" min="4" width="4.5"/>
-    <col customWidth="1" max="5" min="5" width="4.5"/>
-    <col customWidth="1" max="6" min="6" width="4.5"/>
-    <col customWidth="1" max="7" min="7" width="4.5"/>
-    <col customWidth="1" max="8" min="8" width="4.5"/>
-    <col customWidth="1" max="9" min="9" width="4.5"/>
-    <col customWidth="1" max="10" min="10" width="4.5"/>
-    <col customWidth="1" max="11" min="11" width="4.5"/>
-    <col customWidth="1" max="12" min="12" width="4.5"/>
-    <col customWidth="1" max="13" min="13" width="4.5"/>
-    <col customWidth="1" max="14" min="14" width="4.5"/>
-    <col customWidth="1" max="15" min="15" width="4.5"/>
-    <col customWidth="1" max="16" min="16" width="4.5"/>
-    <col customWidth="1" max="17" min="17" width="4.5"/>
-    <col customWidth="1" max="18" min="18" width="4.5"/>
-    <col customWidth="1" max="19" min="19" width="4.5"/>
-    <col customWidth="1" max="20" min="20" width="4.5"/>
-    <col customWidth="1" max="21" min="21" width="4.5"/>
-    <col customWidth="1" max="22" min="22" width="4.5"/>
-    <col customWidth="1" max="23" min="23" width="4.5"/>
-    <col customWidth="1" max="24" min="24" width="4.5"/>
-    <col customWidth="1" max="25" min="25" width="4.5"/>
-    <col customWidth="1" max="26" min="26" width="4.5"/>
-    <col customWidth="1" max="27" min="27" width="4.5"/>
-    <col customWidth="1" max="28" min="28" width="4.5"/>
-    <col customWidth="1" max="29" min="29" width="4.5"/>
-    <col customWidth="1" max="30" min="30" width="4.5"/>
-    <col customWidth="1" max="31" min="31" width="4.5"/>
+    <col width="11.5" customWidth="1" min="1" max="1"/>
+    <col width="4.5" customWidth="1" min="2" max="2"/>
+    <col width="4.5" customWidth="1" min="3" max="3"/>
+    <col width="4.5" customWidth="1" min="4" max="4"/>
+    <col width="4.5" customWidth="1" min="5" max="5"/>
+    <col width="4.5" customWidth="1" min="6" max="6"/>
+    <col width="4.5" customWidth="1" min="7" max="7"/>
+    <col width="4.5" customWidth="1" min="8" max="8"/>
+    <col width="4.5" customWidth="1" min="9" max="9"/>
+    <col width="4.5" customWidth="1" min="10" max="10"/>
+    <col width="4.5" customWidth="1" min="11" max="11"/>
+    <col width="4.5" customWidth="1" min="12" max="12"/>
+    <col width="4.5" customWidth="1" min="13" max="13"/>
+    <col width="4.5" customWidth="1" min="14" max="14"/>
+    <col width="4.5" customWidth="1" min="15" max="15"/>
+    <col width="4.5" customWidth="1" min="16" max="16"/>
+    <col width="4.5" customWidth="1" min="17" max="17"/>
+    <col width="4.5" customWidth="1" min="18" max="18"/>
+    <col width="4.5" customWidth="1" min="19" max="19"/>
+    <col width="4.5" customWidth="1" min="20" max="20"/>
+    <col width="4.5" customWidth="1" min="21" max="21"/>
+    <col width="4.5" customWidth="1" min="22" max="22"/>
+    <col width="4.5" customWidth="1" min="23" max="23"/>
+    <col width="4.5" customWidth="1" min="24" max="24"/>
+    <col width="4.5" customWidth="1" min="25" max="25"/>
+    <col width="4.5" customWidth="1" min="26" max="26"/>
+    <col width="4.5" customWidth="1" min="27" max="27"/>
+    <col width="4.5" customWidth="1" min="28" max="28"/>
+    <col width="4.5" customWidth="1" min="29" max="29"/>
+    <col width="4.5" customWidth="1" min="30" max="30"/>
+    <col width="4.5" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="45" r="1">
+    <row r="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: FEBRUARY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -644,150 +644,150 @@
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="20" r="2">
+    <row r="2" ht="20" customHeight="1">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>CBOC/CORE</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22" r="3">
+    <row r="3" ht="22" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="27" r="4">
+    <row r="4" ht="27" customHeight="1">
       <c r="A4" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="5">
+    <row r="5" ht="21" customHeight="1">
       <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="6">
+    <row r="6" ht="21" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="7">
+    <row r="7" ht="10" customHeight="1">
       <c r="A7" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="8">
+    <row r="8" ht="21" customHeight="1">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="9">
+    <row r="9" ht="21" customHeight="1">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="10">
+    <row r="10" ht="10" customHeight="1">
       <c r="A10" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="11">
+    <row r="11" ht="21" customHeight="1">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="12">
+    <row r="12" ht="21" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="13">
+    <row r="13" ht="10" customHeight="1">
       <c r="A13" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="14">
+    <row r="14" ht="21" customHeight="1">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="15">
+    <row r="15" ht="21" customHeight="1">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="16">
+    <row r="16" ht="10" customHeight="1">
       <c r="A16" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="17">
+    <row r="17" ht="21" customHeight="1">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="18">
+    <row r="18" ht="21" customHeight="1">
       <c r="A18" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="19">
+    <row r="19" ht="10" customHeight="1">
       <c r="A19" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="20">
+    <row r="20" ht="21" customHeight="1">
       <c r="A20" s="7" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="21">
+    <row r="21" ht="21" customHeight="1">
       <c r="A21" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="22">
+    <row r="22" ht="10" customHeight="1">
       <c r="A22" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="23">
+    <row r="23" ht="21" customHeight="1">
       <c r="A23" s="7" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="24">
+    <row r="24" ht="21" customHeight="1">
       <c r="A24" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="25">
+    <row r="25" ht="10" customHeight="1">
       <c r="A25" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="26">
+    <row r="26" ht="21" customHeight="1">
       <c r="A26" s="7" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="27">
+    <row r="27" ht="21" customHeight="1">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Frozen</t>
@@ -798,7 +798,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -808,7 +808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -816,45 +816,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="11.5"/>
-    <col customWidth="1" max="2" min="2" width="4.5"/>
-    <col customWidth="1" max="3" min="3" width="4.5"/>
-    <col customWidth="1" max="4" min="4" width="4.5"/>
-    <col customWidth="1" max="5" min="5" width="4.5"/>
-    <col customWidth="1" max="6" min="6" width="4.5"/>
-    <col customWidth="1" max="7" min="7" width="4.5"/>
-    <col customWidth="1" max="8" min="8" width="4.5"/>
-    <col customWidth="1" max="9" min="9" width="4.5"/>
-    <col customWidth="1" max="10" min="10" width="4.5"/>
-    <col customWidth="1" max="11" min="11" width="4.5"/>
-    <col customWidth="1" max="12" min="12" width="4.5"/>
-    <col customWidth="1" max="13" min="13" width="4.5"/>
-    <col customWidth="1" max="14" min="14" width="4.5"/>
-    <col customWidth="1" max="15" min="15" width="4.5"/>
-    <col customWidth="1" max="16" min="16" width="4.5"/>
-    <col customWidth="1" max="17" min="17" width="4.5"/>
-    <col customWidth="1" max="18" min="18" width="4.5"/>
-    <col customWidth="1" max="19" min="19" width="4.5"/>
-    <col customWidth="1" max="20" min="20" width="4.5"/>
-    <col customWidth="1" max="21" min="21" width="4.5"/>
-    <col customWidth="1" max="22" min="22" width="4.5"/>
-    <col customWidth="1" max="23" min="23" width="4.5"/>
-    <col customWidth="1" max="24" min="24" width="4.5"/>
-    <col customWidth="1" max="25" min="25" width="4.5"/>
-    <col customWidth="1" max="26" min="26" width="4.5"/>
-    <col customWidth="1" max="27" min="27" width="4.5"/>
-    <col customWidth="1" max="28" min="28" width="4.5"/>
-    <col customWidth="1" max="29" min="29" width="4.5"/>
-    <col customWidth="1" max="30" min="30" width="4.5"/>
-    <col customWidth="1" max="31" min="31" width="4.5"/>
-    <col customWidth="1" max="32" min="32" width="4.5"/>
-    <col customWidth="1" max="33" min="33" width="4.5"/>
+    <col width="11.5" customWidth="1" min="1" max="1"/>
+    <col width="4.5" customWidth="1" min="2" max="2"/>
+    <col width="4.5" customWidth="1" min="3" max="3"/>
+    <col width="4.5" customWidth="1" min="4" max="4"/>
+    <col width="4.5" customWidth="1" min="5" max="5"/>
+    <col width="4.5" customWidth="1" min="6" max="6"/>
+    <col width="4.5" customWidth="1" min="7" max="7"/>
+    <col width="4.5" customWidth="1" min="8" max="8"/>
+    <col width="4.5" customWidth="1" min="9" max="9"/>
+    <col width="4.5" customWidth="1" min="10" max="10"/>
+    <col width="4.5" customWidth="1" min="11" max="11"/>
+    <col width="4.5" customWidth="1" min="12" max="12"/>
+    <col width="4.5" customWidth="1" min="13" max="13"/>
+    <col width="4.5" customWidth="1" min="14" max="14"/>
+    <col width="4.5" customWidth="1" min="15" max="15"/>
+    <col width="4.5" customWidth="1" min="16" max="16"/>
+    <col width="4.5" customWidth="1" min="17" max="17"/>
+    <col width="4.5" customWidth="1" min="18" max="18"/>
+    <col width="4.5" customWidth="1" min="19" max="19"/>
+    <col width="4.5" customWidth="1" min="20" max="20"/>
+    <col width="4.5" customWidth="1" min="21" max="21"/>
+    <col width="4.5" customWidth="1" min="22" max="22"/>
+    <col width="4.5" customWidth="1" min="23" max="23"/>
+    <col width="4.5" customWidth="1" min="24" max="24"/>
+    <col width="4.5" customWidth="1" min="25" max="25"/>
+    <col width="4.5" customWidth="1" min="26" max="26"/>
+    <col width="4.5" customWidth="1" min="27" max="27"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="45" r="1">
+    <row r="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: FEBRUARY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -882,158 +876,152 @@
       <c r="X1" s="2" t="n"/>
       <c r="Y1" s="2" t="n"/>
       <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-      <c r="AE1" s="2" t="n"/>
-      <c r="AF1" s="2" t="n"/>
-      <c r="AG1" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="20" r="2">
+      <c r="AA1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="20" customHeight="1">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>CBOC/CORE</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22" r="3">
+    <row r="3" ht="22" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="27" r="4">
+    <row r="4" ht="27" customHeight="1">
       <c r="A4" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="5">
+    <row r="5" ht="21" customHeight="1">
       <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="6">
+    <row r="6" ht="21" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="7">
+    <row r="7" ht="10" customHeight="1">
       <c r="A7" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="8">
+    <row r="8" ht="21" customHeight="1">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="9">
+    <row r="9" ht="21" customHeight="1">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="10">
+    <row r="10" ht="10" customHeight="1">
       <c r="A10" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="11">
+    <row r="11" ht="21" customHeight="1">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="12">
+    <row r="12" ht="21" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="13">
+    <row r="13" ht="10" customHeight="1">
       <c r="A13" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="14">
+    <row r="14" ht="21" customHeight="1">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="15">
+    <row r="15" ht="21" customHeight="1">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="16">
+    <row r="16" ht="10" customHeight="1">
       <c r="A16" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="17">
+    <row r="17" ht="21" customHeight="1">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="18">
+    <row r="18" ht="21" customHeight="1">
       <c r="A18" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="19">
+    <row r="19" ht="10" customHeight="1">
       <c r="A19" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="20">
+    <row r="20" ht="21" customHeight="1">
       <c r="A20" s="7" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="21">
+    <row r="21" ht="21" customHeight="1">
       <c r="A21" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="22">
+    <row r="22" ht="10" customHeight="1">
       <c r="A22" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="23">
+    <row r="23" ht="21" customHeight="1">
       <c r="A23" s="7" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="24">
+    <row r="24" ht="21" customHeight="1">
       <c r="A24" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="10" r="25">
+    <row r="25" ht="10" customHeight="1">
       <c r="A25" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="26">
+    <row r="26" ht="21" customHeight="1">
       <c r="A26" s="7" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="27">
+    <row r="27" ht="21" customHeight="1">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Frozen</t>
@@ -1042,8 +1030,8 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="A1:AA1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dayname and calendar day and week date all working
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="1-15" sheetId="1" state="visible" r:id="rId1"/>
@@ -187,25 +187,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -574,43 +574,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.5" customWidth="1" min="1" max="1"/>
-    <col width="4.5" customWidth="1" min="2" max="2"/>
-    <col width="4.5" customWidth="1" min="3" max="3"/>
-    <col width="4.5" customWidth="1" min="4" max="4"/>
-    <col width="4.5" customWidth="1" min="5" max="5"/>
-    <col width="4.5" customWidth="1" min="6" max="6"/>
-    <col width="4.5" customWidth="1" min="7" max="7"/>
-    <col width="4.5" customWidth="1" min="8" max="8"/>
-    <col width="4.5" customWidth="1" min="9" max="9"/>
-    <col width="4.5" customWidth="1" min="10" max="10"/>
-    <col width="4.5" customWidth="1" min="11" max="11"/>
-    <col width="4.5" customWidth="1" min="12" max="12"/>
-    <col width="4.5" customWidth="1" min="13" max="13"/>
-    <col width="4.5" customWidth="1" min="14" max="14"/>
-    <col width="4.5" customWidth="1" min="15" max="15"/>
-    <col width="4.5" customWidth="1" min="16" max="16"/>
-    <col width="4.5" customWidth="1" min="17" max="17"/>
-    <col width="4.5" customWidth="1" min="18" max="18"/>
-    <col width="4.5" customWidth="1" min="19" max="19"/>
-    <col width="4.5" customWidth="1" min="20" max="20"/>
-    <col width="4.5" customWidth="1" min="21" max="21"/>
-    <col width="4.5" customWidth="1" min="22" max="22"/>
-    <col width="4.5" customWidth="1" min="23" max="23"/>
-    <col width="4.5" customWidth="1" min="24" max="24"/>
-    <col width="4.5" customWidth="1" min="25" max="25"/>
-    <col width="4.5" customWidth="1" min="26" max="26"/>
-    <col width="4.5" customWidth="1" min="27" max="27"/>
-    <col width="4.5" customWidth="1" min="28" max="28"/>
-    <col width="4.5" customWidth="1" min="29" max="29"/>
-    <col width="4.5" customWidth="1" min="30" max="30"/>
-    <col width="4.5" customWidth="1" min="31" max="31"/>
+    <col customWidth="1" max="1" min="1" width="11.5"/>
+    <col customWidth="1" max="2" min="2" width="4.5"/>
+    <col customWidth="1" max="3" min="3" width="4.5"/>
+    <col customWidth="1" max="4" min="4" width="4.5"/>
+    <col customWidth="1" max="5" min="5" width="4.5"/>
+    <col customWidth="1" max="6" min="6" width="4.5"/>
+    <col customWidth="1" max="7" min="7" width="4.5"/>
+    <col customWidth="1" max="8" min="8" width="4.5"/>
+    <col customWidth="1" max="9" min="9" width="4.5"/>
+    <col customWidth="1" max="10" min="10" width="4.5"/>
+    <col customWidth="1" max="11" min="11" width="4.5"/>
+    <col customWidth="1" max="12" min="12" width="4.5"/>
+    <col customWidth="1" max="13" min="13" width="4.5"/>
+    <col customWidth="1" max="14" min="14" width="4.5"/>
+    <col customWidth="1" max="15" min="15" width="4.5"/>
+    <col customWidth="1" max="16" min="16" width="4.5"/>
+    <col customWidth="1" max="17" min="17" width="4.5"/>
+    <col customWidth="1" max="18" min="18" width="4.5"/>
+    <col customWidth="1" max="19" min="19" width="4.5"/>
+    <col customWidth="1" max="20" min="20" width="4.5"/>
+    <col customWidth="1" max="21" min="21" width="4.5"/>
+    <col customWidth="1" max="22" min="22" width="4.5"/>
+    <col customWidth="1" max="23" min="23" width="4.5"/>
+    <col customWidth="1" max="24" min="24" width="4.5"/>
+    <col customWidth="1" max="25" min="25" width="4.5"/>
+    <col customWidth="1" max="26" min="26" width="4.5"/>
+    <col customWidth="1" max="27" min="27" width="4.5"/>
+    <col customWidth="1" max="28" min="28" width="4.5"/>
+    <col customWidth="1" max="29" min="29" width="4.5"/>
+    <col customWidth="1" max="30" min="30" width="4.5"/>
+    <col customWidth="1" max="31" min="31" width="4.5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2021</t>
+          <t>Month/Year: MAY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -644,150 +644,150 @@
       <c r="AD1" s="2" t="n"/>
       <c r="AE1" s="3" t="n"/>
     </row>
-    <row r="2" ht="20" customHeight="1">
+    <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>CBOC/CORE</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="22" customHeight="1">
+    <row customHeight="1" ht="22" r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="27" customHeight="1">
+    <row customHeight="1" ht="27" r="4">
       <c r="A4" s="6" t="n"/>
     </row>
-    <row r="5" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="6">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="7">
       <c r="A7" s="6" t="n"/>
     </row>
-    <row r="8" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="8">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="10">
       <c r="A10" s="6" t="n"/>
     </row>
-    <row r="11" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="11">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="12">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="13">
       <c r="A13" s="6" t="n"/>
     </row>
-    <row r="14" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="14">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="15">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="16">
       <c r="A16" s="6" t="n"/>
     </row>
-    <row r="17" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="17">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="19" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="19">
       <c r="A19" s="6" t="n"/>
     </row>
-    <row r="20" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="20">
       <c r="A20" s="7" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="22">
       <c r="A22" s="6" t="n"/>
     </row>
-    <row r="23" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="23">
       <c r="A23" s="7" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="24">
       <c r="A24" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="25">
       <c r="A25" s="6" t="n"/>
     </row>
-    <row r="26" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="26">
       <c r="A26" s="7" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Frozen</t>
@@ -798,7 +798,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AE1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -808,7 +808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AG27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -816,39 +816,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.5" customWidth="1" min="1" max="1"/>
-    <col width="4.5" customWidth="1" min="2" max="2"/>
-    <col width="4.5" customWidth="1" min="3" max="3"/>
-    <col width="4.5" customWidth="1" min="4" max="4"/>
-    <col width="4.5" customWidth="1" min="5" max="5"/>
-    <col width="4.5" customWidth="1" min="6" max="6"/>
-    <col width="4.5" customWidth="1" min="7" max="7"/>
-    <col width="4.5" customWidth="1" min="8" max="8"/>
-    <col width="4.5" customWidth="1" min="9" max="9"/>
-    <col width="4.5" customWidth="1" min="10" max="10"/>
-    <col width="4.5" customWidth="1" min="11" max="11"/>
-    <col width="4.5" customWidth="1" min="12" max="12"/>
-    <col width="4.5" customWidth="1" min="13" max="13"/>
-    <col width="4.5" customWidth="1" min="14" max="14"/>
-    <col width="4.5" customWidth="1" min="15" max="15"/>
-    <col width="4.5" customWidth="1" min="16" max="16"/>
-    <col width="4.5" customWidth="1" min="17" max="17"/>
-    <col width="4.5" customWidth="1" min="18" max="18"/>
-    <col width="4.5" customWidth="1" min="19" max="19"/>
-    <col width="4.5" customWidth="1" min="20" max="20"/>
-    <col width="4.5" customWidth="1" min="21" max="21"/>
-    <col width="4.5" customWidth="1" min="22" max="22"/>
-    <col width="4.5" customWidth="1" min="23" max="23"/>
-    <col width="4.5" customWidth="1" min="24" max="24"/>
-    <col width="4.5" customWidth="1" min="25" max="25"/>
-    <col width="4.5" customWidth="1" min="26" max="26"/>
-    <col width="4.5" customWidth="1" min="27" max="27"/>
+    <col customWidth="1" max="1" min="1" width="11.5"/>
+    <col customWidth="1" max="2" min="2" width="4.5"/>
+    <col customWidth="1" max="3" min="3" width="4.5"/>
+    <col customWidth="1" max="4" min="4" width="4.5"/>
+    <col customWidth="1" max="5" min="5" width="4.5"/>
+    <col customWidth="1" max="6" min="6" width="4.5"/>
+    <col customWidth="1" max="7" min="7" width="4.5"/>
+    <col customWidth="1" max="8" min="8" width="4.5"/>
+    <col customWidth="1" max="9" min="9" width="4.5"/>
+    <col customWidth="1" max="10" min="10" width="4.5"/>
+    <col customWidth="1" max="11" min="11" width="4.5"/>
+    <col customWidth="1" max="12" min="12" width="4.5"/>
+    <col customWidth="1" max="13" min="13" width="4.5"/>
+    <col customWidth="1" max="14" min="14" width="4.5"/>
+    <col customWidth="1" max="15" min="15" width="4.5"/>
+    <col customWidth="1" max="16" min="16" width="4.5"/>
+    <col customWidth="1" max="17" min="17" width="4.5"/>
+    <col customWidth="1" max="18" min="18" width="4.5"/>
+    <col customWidth="1" max="19" min="19" width="4.5"/>
+    <col customWidth="1" max="20" min="20" width="4.5"/>
+    <col customWidth="1" max="21" min="21" width="4.5"/>
+    <col customWidth="1" max="22" min="22" width="4.5"/>
+    <col customWidth="1" max="23" min="23" width="4.5"/>
+    <col customWidth="1" max="24" min="24" width="4.5"/>
+    <col customWidth="1" max="25" min="25" width="4.5"/>
+    <col customWidth="1" max="26" min="26" width="4.5"/>
+    <col customWidth="1" max="27" min="27" width="4.5"/>
+    <col customWidth="1" max="28" min="28" width="4.5"/>
+    <col customWidth="1" max="29" min="29" width="4.5"/>
+    <col customWidth="1" max="30" min="30" width="4.5"/>
+    <col customWidth="1" max="31" min="31" width="4.5"/>
+    <col customWidth="1" max="32" min="32" width="4.5"/>
+    <col customWidth="1" max="33" min="33" width="4.5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2021</t>
+          <t>Month/Year: MAY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -876,152 +882,158 @@
       <c r="X1" s="2" t="n"/>
       <c r="Y1" s="2" t="n"/>
       <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="20" customHeight="1">
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>CBOC/CORE</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="22" customHeight="1">
+    <row customHeight="1" ht="22" r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="27" customHeight="1">
+    <row customHeight="1" ht="27" r="4">
       <c r="A4" s="6" t="n"/>
     </row>
-    <row r="5" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="6">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="7">
       <c r="A7" s="6" t="n"/>
     </row>
-    <row r="8" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="8">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="10">
       <c r="A10" s="6" t="n"/>
     </row>
-    <row r="11" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="11">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="12">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="13">
       <c r="A13" s="6" t="n"/>
     </row>
-    <row r="14" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="14">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="15">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="16">
       <c r="A16" s="6" t="n"/>
     </row>
-    <row r="17" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="17">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="19" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="19">
       <c r="A19" s="6" t="n"/>
     </row>
-    <row r="20" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="20">
       <c r="A20" s="7" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="22">
       <c r="A22" s="6" t="n"/>
     </row>
-    <row r="23" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="23">
       <c r="A23" s="7" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="24">
       <c r="A24" s="8" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="10" customHeight="1">
+    <row customHeight="1" ht="10" r="25">
       <c r="A25" s="6" t="n"/>
     </row>
-    <row r="26" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="26">
       <c r="A26" s="7" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="21" customHeight="1">
+    <row customHeight="1" ht="21" r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Frozen</t>
@@ -1030,8 +1042,8 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A1:AG1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
date nums and day names working correctly!!
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,6 +30,11 @@
       <name val="Times New Roman"/>
       <b val="1"/>
       <sz val="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="10"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -189,14 +194,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -610,7 +618,7 @@
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: FEBRUARY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -650,145 +658,265 @@
           <t>CBOC/CORE</t>
         </is>
       </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>TUE</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>WED</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>THU</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>FRI</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>SAT</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>SUN</t>
+        </is>
+      </c>
+      <c r="P2" s="5" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="R2" s="5" t="inlineStr">
+        <is>
+          <t>TUE</t>
+        </is>
+      </c>
+      <c r="T2" s="5" t="inlineStr">
+        <is>
+          <t>WED</t>
+        </is>
+      </c>
+      <c r="V2" s="5" t="inlineStr">
+        <is>
+          <t>THU</t>
+        </is>
+      </c>
+      <c r="X2" s="5" t="inlineStr">
+        <is>
+          <t>FRI</t>
+        </is>
+      </c>
+      <c r="Z2" s="5" t="inlineStr">
+        <is>
+          <t>SAT</t>
+        </is>
+      </c>
+      <c r="AB2" s="5" t="inlineStr">
+        <is>
+          <t>SUN</t>
+        </is>
+      </c>
+      <c r="AD2" s="5" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="22" r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
+      <c r="B3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="P3" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="R3" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="T3" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="V3" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="X3" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="AB3" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD3" s="5" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row customHeight="1" ht="27" r="4">
-      <c r="A4" s="6" t="n"/>
+      <c r="A4" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="8" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="6">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="7">
-      <c r="A7" s="6" t="n"/>
+      <c r="A7" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
-      <c r="A8" s="7" t="inlineStr">
+      <c r="A8" s="8" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="9">
-      <c r="A9" s="8" t="inlineStr">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="10">
-      <c r="A10" s="6" t="n"/>
+      <c r="A10" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="8" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="12">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="A12" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="13">
-      <c r="A13" s="6" t="n"/>
+      <c r="A13" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
-      <c r="A14" s="7" t="inlineStr">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="15">
-      <c r="A15" s="8" t="inlineStr">
+      <c r="A15" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="16">
-      <c r="A16" s="6" t="n"/>
+      <c r="A16" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
-      <c r="A17" s="7" t="inlineStr">
+      <c r="A17" s="8" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="18">
-      <c r="A18" s="8" t="inlineStr">
+      <c r="A18" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="19">
-      <c r="A19" s="6" t="n"/>
+      <c r="A19" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
-      <c r="A20" s="7" t="inlineStr">
+      <c r="A20" s="8" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="21">
-      <c r="A21" s="8" t="inlineStr">
+      <c r="A21" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="22">
-      <c r="A22" s="6" t="n"/>
+      <c r="A22" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
-      <c r="A23" s="7" t="inlineStr">
+      <c r="A23" s="8" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="24">
-      <c r="A24" s="8" t="inlineStr">
+      <c r="A24" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="25">
-      <c r="A25" s="6" t="n"/>
+      <c r="A25" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
-      <c r="A26" s="7" t="inlineStr">
+      <c r="A26" s="8" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="27">
-      <c r="A27" s="5" t="inlineStr">
+      <c r="A27" s="6" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -808,7 +936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -843,18 +971,12 @@
     <col customWidth="1" max="25" min="25" width="4.5"/>
     <col customWidth="1" max="26" min="26" width="4.5"/>
     <col customWidth="1" max="27" min="27" width="4.5"/>
-    <col customWidth="1" max="28" min="28" width="4.5"/>
-    <col customWidth="1" max="29" min="29" width="4.5"/>
-    <col customWidth="1" max="30" min="30" width="4.5"/>
-    <col customWidth="1" max="31" min="31" width="4.5"/>
-    <col customWidth="1" max="32" min="32" width="4.5"/>
-    <col customWidth="1" max="33" min="33" width="4.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: FEBRUARY 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -882,13 +1004,7 @@
       <c r="X1" s="2" t="n"/>
       <c r="Y1" s="2" t="n"/>
       <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-      <c r="AE1" s="2" t="n"/>
-      <c r="AF1" s="2" t="n"/>
-      <c r="AG1" s="3" t="n"/>
+      <c r="AA1" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
@@ -896,145 +1012,249 @@
           <t>CBOC/CORE</t>
         </is>
       </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>TUE</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>WED</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>THU</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>FRI</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>SAT</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>SUN</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="P2" s="5" t="inlineStr">
+        <is>
+          <t>TUE</t>
+        </is>
+      </c>
+      <c r="R2" s="5" t="inlineStr">
+        <is>
+          <t>WED</t>
+        </is>
+      </c>
+      <c r="T2" s="5" t="inlineStr">
+        <is>
+          <t>THU</t>
+        </is>
+      </c>
+      <c r="V2" s="5" t="inlineStr">
+        <is>
+          <t>FRI</t>
+        </is>
+      </c>
+      <c r="X2" s="5" t="inlineStr">
+        <is>
+          <t>SAT</t>
+        </is>
+      </c>
+      <c r="Z2" s="5" t="inlineStr">
+        <is>
+          <t>SUN</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="22" r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
+      <c r="B3" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="P3" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="R3" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="T3" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="V3" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="X3" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="Z3" s="5" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row customHeight="1" ht="27" r="4">
-      <c r="A4" s="6" t="n"/>
+      <c r="A4" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="8" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="6">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="7">
-      <c r="A7" s="6" t="n"/>
+      <c r="A7" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
-      <c r="A8" s="7" t="inlineStr">
+      <c r="A8" s="8" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="9">
-      <c r="A9" s="8" t="inlineStr">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="10">
-      <c r="A10" s="6" t="n"/>
+      <c r="A10" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="8" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="12">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="A12" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="13">
-      <c r="A13" s="6" t="n"/>
+      <c r="A13" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
-      <c r="A14" s="7" t="inlineStr">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="15">
-      <c r="A15" s="8" t="inlineStr">
+      <c r="A15" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="16">
-      <c r="A16" s="6" t="n"/>
+      <c r="A16" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
-      <c r="A17" s="7" t="inlineStr">
+      <c r="A17" s="8" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="18">
-      <c r="A18" s="8" t="inlineStr">
+      <c r="A18" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="19">
-      <c r="A19" s="6" t="n"/>
+      <c r="A19" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
-      <c r="A20" s="7" t="inlineStr">
+      <c r="A20" s="8" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="21">
-      <c r="A21" s="8" t="inlineStr">
+      <c r="A21" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="22">
-      <c r="A22" s="6" t="n"/>
+      <c r="A22" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
-      <c r="A23" s="7" t="inlineStr">
+      <c r="A23" s="8" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="24">
-      <c r="A24" s="8" t="inlineStr">
+      <c r="A24" s="9" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="25">
-      <c r="A25" s="6" t="n"/>
+      <c r="A25" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
-      <c r="A26" s="7" t="inlineStr">
+      <c r="A26" s="8" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="27">
-      <c r="A27" s="5" t="inlineStr">
+      <c r="A27" s="6" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1042,7 +1262,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="A1:AA1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
with tech/toa info added and working
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,12 +29,20 @@
     <font>
       <name val="Times New Roman"/>
       <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <sz val="9"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="10"/>
+      <sz val="5"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -194,9 +202,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -207,6 +215,10 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -582,7 +594,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="11.5"/>
+    <col customWidth="1" max="1" min="1" width="12.5"/>
     <col customWidth="1" max="2" min="2" width="4.5"/>
     <col customWidth="1" max="3" min="3" width="4.5"/>
     <col customWidth="1" max="4" min="4" width="4.5"/>
@@ -618,7 +630,7 @@
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2021</t>
+          <t>Month/Year: APRIL 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -660,77 +672,77 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
+          <t>THU</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>FRI</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>SAT</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>SUN</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
           <t>MON</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>TUE</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="N2" s="5" t="inlineStr">
         <is>
           <t>WED</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="P2" s="5" t="inlineStr">
         <is>
           <t>THU</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="R2" s="5" t="inlineStr">
         <is>
           <t>FRI</t>
         </is>
       </c>
-      <c r="L2" s="5" t="inlineStr">
+      <c r="T2" s="5" t="inlineStr">
         <is>
           <t>SAT</t>
         </is>
       </c>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="V2" s="5" t="inlineStr">
         <is>
           <t>SUN</t>
         </is>
       </c>
-      <c r="P2" s="5" t="inlineStr">
+      <c r="X2" s="5" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
-      <c r="R2" s="5" t="inlineStr">
+      <c r="Z2" s="5" t="inlineStr">
         <is>
           <t>TUE</t>
         </is>
       </c>
-      <c r="T2" s="5" t="inlineStr">
+      <c r="AB2" s="5" t="inlineStr">
         <is>
           <t>WED</t>
         </is>
       </c>
-      <c r="V2" s="5" t="inlineStr">
+      <c r="AD2" s="5" t="inlineStr">
         <is>
           <t>THU</t>
-        </is>
-      </c>
-      <c r="X2" s="5" t="inlineStr">
-        <is>
-          <t>FRI</t>
-        </is>
-      </c>
-      <c r="Z2" s="5" t="inlineStr">
-        <is>
-          <t>SAT</t>
-        </is>
-      </c>
-      <c r="AB2" s="5" t="inlineStr">
-        <is>
-          <t>SUN</t>
-        </is>
-      </c>
-      <c r="AD2" s="5" t="inlineStr">
-        <is>
-          <t>MON</t>
         </is>
       </c>
     </row>
@@ -788,16 +800,166 @@
     </row>
     <row customHeight="1" ht="27" r="4">
       <c r="A4" s="7" t="n"/>
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="F4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="G4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="H4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="I4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="K4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="L4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="M4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="N4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="O4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="P4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="Q4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="R4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="S4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="T4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="U4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="V4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="W4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="X4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="Y4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="Z4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AA4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AB4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AC4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AD4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AE4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="5">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="6">
-      <c r="A6" s="9" t="inlineStr">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -807,14 +969,14 @@
       <c r="A7" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="9">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="A9" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -824,14 +986,14 @@
       <c r="A10" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
-      <c r="A11" s="8" t="inlineStr">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="12">
-      <c r="A12" s="9" t="inlineStr">
+      <c r="A12" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -841,14 +1003,14 @@
       <c r="A13" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
-      <c r="A14" s="8" t="inlineStr">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="15">
-      <c r="A15" s="9" t="inlineStr">
+      <c r="A15" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -858,14 +1020,14 @@
       <c r="A16" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
-      <c r="A17" s="8" t="inlineStr">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="18">
-      <c r="A18" s="9" t="inlineStr">
+      <c r="A18" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -875,14 +1037,14 @@
       <c r="A19" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
-      <c r="A20" s="8" t="inlineStr">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="21">
-      <c r="A21" s="9" t="inlineStr">
+      <c r="A21" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -892,14 +1054,14 @@
       <c r="A22" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
-      <c r="A23" s="8" t="inlineStr">
+      <c r="A23" s="10" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="24">
-      <c r="A24" s="9" t="inlineStr">
+      <c r="A24" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -909,7 +1071,7 @@
       <c r="A25" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
-      <c r="A26" s="8" t="inlineStr">
+      <c r="A26" s="10" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
@@ -936,7 +1098,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -944,7 +1106,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="11.5"/>
+    <col customWidth="1" max="1" min="1" width="12.5"/>
     <col customWidth="1" max="2" min="2" width="4.5"/>
     <col customWidth="1" max="3" min="3" width="4.5"/>
     <col customWidth="1" max="4" min="4" width="4.5"/>
@@ -971,12 +1133,16 @@
     <col customWidth="1" max="25" min="25" width="4.5"/>
     <col customWidth="1" max="26" min="26" width="4.5"/>
     <col customWidth="1" max="27" min="27" width="4.5"/>
+    <col customWidth="1" max="28" min="28" width="4.5"/>
+    <col customWidth="1" max="29" min="29" width="4.5"/>
+    <col customWidth="1" max="30" min="30" width="4.5"/>
+    <col customWidth="1" max="31" min="31" width="4.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: FEBRUARY 2021</t>
+          <t>Month/Year: APRIL 2021</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -1004,7 +1170,11 @@
       <c r="X1" s="2" t="n"/>
       <c r="Y1" s="2" t="n"/>
       <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="3" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="20" r="2">
       <c r="A2" s="4" t="inlineStr">
@@ -1014,67 +1184,77 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
+          <t>FRI</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>SAT</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>SUN</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
           <t>TUE</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>WED</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="N2" s="5" t="inlineStr">
         <is>
           <t>THU</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="P2" s="5" t="inlineStr">
         <is>
           <t>FRI</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="R2" s="5" t="inlineStr">
         <is>
           <t>SAT</t>
         </is>
       </c>
-      <c r="L2" s="5" t="inlineStr">
+      <c r="T2" s="5" t="inlineStr">
         <is>
           <t>SUN</t>
         </is>
       </c>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="V2" s="5" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
-      <c r="P2" s="5" t="inlineStr">
+      <c r="X2" s="5" t="inlineStr">
         <is>
           <t>TUE</t>
         </is>
       </c>
-      <c r="R2" s="5" t="inlineStr">
+      <c r="Z2" s="5" t="inlineStr">
         <is>
           <t>WED</t>
         </is>
       </c>
-      <c r="T2" s="5" t="inlineStr">
+      <c r="AB2" s="5" t="inlineStr">
         <is>
           <t>THU</t>
         </is>
       </c>
-      <c r="V2" s="5" t="inlineStr">
+      <c r="AD2" s="5" t="inlineStr">
         <is>
           <t>FRI</t>
-        </is>
-      </c>
-      <c r="X2" s="5" t="inlineStr">
-        <is>
-          <t>SAT</t>
-        </is>
-      </c>
-      <c r="Z2" s="5" t="inlineStr">
-        <is>
-          <t>SUN</t>
         </is>
       </c>
     </row>
@@ -1123,19 +1303,175 @@
       <c r="Z3" s="5" t="n">
         <v>28</v>
       </c>
+      <c r="AB3" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD3" s="5" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row customHeight="1" ht="27" r="4">
       <c r="A4" s="7" t="n"/>
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="F4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="G4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="H4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="I4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="K4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="L4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="M4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="N4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="O4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="P4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="Q4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="R4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="S4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="T4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="U4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="V4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="W4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="X4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="Y4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="Z4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AA4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AB4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AC4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AD4" s="8" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AE4" s="9" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="5">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="6">
-      <c r="A6" s="9" t="inlineStr">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1145,14 +1481,14 @@
       <c r="A7" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="9">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="A9" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1162,14 +1498,14 @@
       <c r="A10" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
-      <c r="A11" s="8" t="inlineStr">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="12">
-      <c r="A12" s="9" t="inlineStr">
+      <c r="A12" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1179,14 +1515,14 @@
       <c r="A13" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
-      <c r="A14" s="8" t="inlineStr">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="15">
-      <c r="A15" s="9" t="inlineStr">
+      <c r="A15" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1196,14 +1532,14 @@
       <c r="A16" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
-      <c r="A17" s="8" t="inlineStr">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="18">
-      <c r="A18" s="9" t="inlineStr">
+      <c r="A18" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1213,14 +1549,14 @@
       <c r="A19" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
-      <c r="A20" s="8" t="inlineStr">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="21">
-      <c r="A21" s="9" t="inlineStr">
+      <c r="A21" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1230,14 +1566,14 @@
       <c r="A22" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
-      <c r="A23" s="8" t="inlineStr">
+      <c r="A23" s="10" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="24">
-      <c r="A24" s="9" t="inlineStr">
+      <c r="A24" s="11" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1247,7 +1583,7 @@
       <c r="A25" s="7" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
-      <c r="A26" s="8" t="inlineStr">
+      <c r="A26" s="10" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
@@ -1262,7 +1598,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A1:AE1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
with date info borders working even for merged cells
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -202,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -210,9 +210,10 @@
     <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -675,79 +676,94 @@
           <t>SAT</t>
         </is>
       </c>
+      <c r="C2" s="6" t="n"/>
       <c r="D2" s="5" t="inlineStr">
         <is>
           <t>SUN</t>
         </is>
       </c>
+      <c r="E2" s="6" t="n"/>
       <c r="F2" s="5" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
+      <c r="G2" s="6" t="n"/>
       <c r="H2" s="5" t="inlineStr">
         <is>
           <t>TUE</t>
         </is>
       </c>
+      <c r="I2" s="6" t="n"/>
       <c r="J2" s="5" t="inlineStr">
         <is>
           <t>WED</t>
         </is>
       </c>
+      <c r="K2" s="6" t="n"/>
       <c r="L2" s="5" t="inlineStr">
         <is>
           <t>THU</t>
         </is>
       </c>
+      <c r="M2" s="6" t="n"/>
       <c r="N2" s="5" t="inlineStr">
         <is>
           <t>FRI</t>
         </is>
       </c>
+      <c r="O2" s="6" t="n"/>
       <c r="P2" s="5" t="inlineStr">
         <is>
           <t>SAT</t>
         </is>
       </c>
+      <c r="Q2" s="6" t="n"/>
       <c r="R2" s="5" t="inlineStr">
         <is>
           <t>SUN</t>
         </is>
       </c>
+      <c r="S2" s="6" t="n"/>
       <c r="T2" s="5" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
+      <c r="U2" s="6" t="n"/>
       <c r="V2" s="5" t="inlineStr">
         <is>
           <t>TUE</t>
         </is>
       </c>
+      <c r="W2" s="6" t="n"/>
       <c r="X2" s="5" t="inlineStr">
         <is>
           <t>WED</t>
         </is>
       </c>
+      <c r="Y2" s="6" t="n"/>
       <c r="Z2" s="5" t="inlineStr">
         <is>
           <t>THU</t>
         </is>
       </c>
+      <c r="AA2" s="6" t="n"/>
       <c r="AB2" s="5" t="inlineStr">
         <is>
           <t>FRI</t>
         </is>
       </c>
+      <c r="AC2" s="6" t="n"/>
       <c r="AD2" s="5" t="inlineStr">
         <is>
           <t>SAT</t>
         </is>
       </c>
+      <c r="AE2" s="6" t="n"/>
     </row>
     <row customHeight="1" ht="22" r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
@@ -755,330 +771,345 @@
       <c r="B3" s="5" t="n">
         <v>1</v>
       </c>
+      <c r="C3" s="6" t="n"/>
       <c r="D3" s="5" t="n">
         <v>2</v>
       </c>
+      <c r="E3" s="6" t="n"/>
       <c r="F3" s="5" t="n">
         <v>3</v>
       </c>
+      <c r="G3" s="6" t="n"/>
       <c r="H3" s="5" t="n">
         <v>4</v>
       </c>
+      <c r="I3" s="6" t="n"/>
       <c r="J3" s="5" t="n">
         <v>5</v>
       </c>
+      <c r="K3" s="6" t="n"/>
       <c r="L3" s="5" t="n">
         <v>6</v>
       </c>
+      <c r="M3" s="6" t="n"/>
       <c r="N3" s="5" t="n">
         <v>7</v>
       </c>
+      <c r="O3" s="6" t="n"/>
       <c r="P3" s="5" t="n">
         <v>8</v>
       </c>
+      <c r="Q3" s="6" t="n"/>
       <c r="R3" s="5" t="n">
         <v>9</v>
       </c>
+      <c r="S3" s="6" t="n"/>
       <c r="T3" s="5" t="n">
         <v>10</v>
       </c>
+      <c r="U3" s="6" t="n"/>
       <c r="V3" s="5" t="n">
         <v>11</v>
       </c>
+      <c r="W3" s="6" t="n"/>
       <c r="X3" s="5" t="n">
         <v>12</v>
       </c>
+      <c r="Y3" s="6" t="n"/>
       <c r="Z3" s="5" t="n">
         <v>13</v>
       </c>
+      <c r="AA3" s="6" t="n"/>
       <c r="AB3" s="5" t="n">
         <v>14</v>
       </c>
+      <c r="AC3" s="6" t="n"/>
       <c r="AD3" s="5" t="n">
         <v>15</v>
       </c>
+      <c r="AE3" s="6" t="n"/>
     </row>
     <row customHeight="1" ht="27" r="4">
-      <c r="A4" s="7" t="n"/>
-      <c r="B4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="D4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="F4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="G4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="H4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="I4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="J4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="K4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="L4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="M4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="N4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="O4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="P4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="Q4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="R4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="S4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="T4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="U4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="V4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="W4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="X4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="Y4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="Z4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="AA4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="AB4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="AC4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="AD4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="AE4" s="9" t="inlineStr">
+      <c r="A4" s="8" t="n"/>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="C4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="F4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="H4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="I4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="J4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="K4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="L4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="M4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="N4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="O4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="P4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="Q4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="R4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="S4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="T4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="U4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="V4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="W4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="X4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="Y4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="Z4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AA4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AB4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AC4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AD4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AE4" s="10" t="inlineStr">
         <is>
           <t>Time of Arrival</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="5">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="6">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="A6" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="7">
-      <c r="A7" s="7" t="n"/>
+      <c r="A7" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="A8" s="11" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="9">
-      <c r="A9" s="11" t="inlineStr">
+      <c r="A9" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="10">
-      <c r="A10" s="7" t="n"/>
+      <c r="A10" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
-      <c r="A11" s="10" t="inlineStr">
+      <c r="A11" s="11" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="12">
-      <c r="A12" s="11" t="inlineStr">
+      <c r="A12" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="13">
-      <c r="A13" s="7" t="n"/>
+      <c r="A13" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
-      <c r="A14" s="10" t="inlineStr">
+      <c r="A14" s="11" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="15">
-      <c r="A15" s="11" t="inlineStr">
+      <c r="A15" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="16">
-      <c r="A16" s="7" t="n"/>
+      <c r="A16" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
-      <c r="A17" s="10" t="inlineStr">
+      <c r="A17" s="11" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="18">
-      <c r="A18" s="11" t="inlineStr">
+      <c r="A18" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="19">
-      <c r="A19" s="7" t="n"/>
+      <c r="A19" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
-      <c r="A20" s="10" t="inlineStr">
+      <c r="A20" s="11" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="21">
-      <c r="A21" s="11" t="inlineStr">
+      <c r="A21" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="22">
-      <c r="A22" s="7" t="n"/>
+      <c r="A22" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
-      <c r="A23" s="10" t="inlineStr">
+      <c r="A23" s="11" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="24">
-      <c r="A24" s="11" t="inlineStr">
+      <c r="A24" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="25">
-      <c r="A25" s="7" t="n"/>
+      <c r="A25" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
-      <c r="A26" s="10" t="inlineStr">
+      <c r="A26" s="11" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="27">
-      <c r="A27" s="6" t="inlineStr">
+      <c r="A27" s="7" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
@@ -1221,84 +1252,100 @@
           <t>SUN</t>
         </is>
       </c>
+      <c r="C2" s="6" t="n"/>
       <c r="D2" s="5" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
+      <c r="E2" s="6" t="n"/>
       <c r="F2" s="5" t="inlineStr">
         <is>
           <t>TUE</t>
         </is>
       </c>
+      <c r="G2" s="6" t="n"/>
       <c r="H2" s="5" t="inlineStr">
         <is>
           <t>WED</t>
         </is>
       </c>
+      <c r="I2" s="6" t="n"/>
       <c r="J2" s="5" t="inlineStr">
         <is>
           <t>THU</t>
         </is>
       </c>
+      <c r="K2" s="6" t="n"/>
       <c r="L2" s="5" t="inlineStr">
         <is>
           <t>FRI</t>
         </is>
       </c>
+      <c r="M2" s="6" t="n"/>
       <c r="N2" s="5" t="inlineStr">
         <is>
           <t>SAT</t>
         </is>
       </c>
+      <c r="O2" s="6" t="n"/>
       <c r="P2" s="5" t="inlineStr">
         <is>
           <t>SUN</t>
         </is>
       </c>
+      <c r="Q2" s="6" t="n"/>
       <c r="R2" s="5" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
+      <c r="S2" s="6" t="n"/>
       <c r="T2" s="5" t="inlineStr">
         <is>
           <t>TUE</t>
         </is>
       </c>
+      <c r="U2" s="6" t="n"/>
       <c r="V2" s="5" t="inlineStr">
         <is>
           <t>WED</t>
         </is>
       </c>
+      <c r="W2" s="6" t="n"/>
       <c r="X2" s="5" t="inlineStr">
         <is>
           <t>THU</t>
         </is>
       </c>
+      <c r="Y2" s="6" t="n"/>
       <c r="Z2" s="5" t="inlineStr">
         <is>
           <t>FRI</t>
         </is>
       </c>
+      <c r="AA2" s="6" t="n"/>
       <c r="AB2" s="5" t="inlineStr">
         <is>
           <t>SAT</t>
         </is>
       </c>
+      <c r="AC2" s="6" t="n"/>
       <c r="AD2" s="5" t="inlineStr">
         <is>
           <t>SUN</t>
         </is>
       </c>
+      <c r="AE2" s="6" t="n"/>
       <c r="AF2" s="5" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
+      <c r="AG2" s="6" t="n"/>
     </row>
     <row customHeight="1" ht="22" r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
@@ -1306,343 +1353,359 @@
       <c r="B3" s="5" t="n">
         <v>16</v>
       </c>
+      <c r="C3" s="6" t="n"/>
       <c r="D3" s="5" t="n">
         <v>17</v>
       </c>
+      <c r="E3" s="6" t="n"/>
       <c r="F3" s="5" t="n">
         <v>18</v>
       </c>
+      <c r="G3" s="6" t="n"/>
       <c r="H3" s="5" t="n">
         <v>19</v>
       </c>
+      <c r="I3" s="6" t="n"/>
       <c r="J3" s="5" t="n">
         <v>20</v>
       </c>
+      <c r="K3" s="6" t="n"/>
       <c r="L3" s="5" t="n">
         <v>21</v>
       </c>
+      <c r="M3" s="6" t="n"/>
       <c r="N3" s="5" t="n">
         <v>22</v>
       </c>
+      <c r="O3" s="6" t="n"/>
       <c r="P3" s="5" t="n">
         <v>23</v>
       </c>
+      <c r="Q3" s="6" t="n"/>
       <c r="R3" s="5" t="n">
         <v>24</v>
       </c>
+      <c r="S3" s="6" t="n"/>
       <c r="T3" s="5" t="n">
         <v>25</v>
       </c>
+      <c r="U3" s="6" t="n"/>
       <c r="V3" s="5" t="n">
         <v>26</v>
       </c>
+      <c r="W3" s="6" t="n"/>
       <c r="X3" s="5" t="n">
         <v>27</v>
       </c>
+      <c r="Y3" s="6" t="n"/>
       <c r="Z3" s="5" t="n">
         <v>28</v>
       </c>
+      <c r="AA3" s="6" t="n"/>
       <c r="AB3" s="5" t="n">
         <v>29</v>
       </c>
+      <c r="AC3" s="6" t="n"/>
       <c r="AD3" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="AE3" s="6" t="n"/>
       <c r="AF3" s="5" t="n">
         <v>31</v>
       </c>
+      <c r="AG3" s="6" t="n"/>
     </row>
     <row customHeight="1" ht="27" r="4">
-      <c r="A4" s="7" t="n"/>
-      <c r="B4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="D4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="F4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="G4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="H4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="I4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="J4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="K4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="L4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="M4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="N4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="O4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="P4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="Q4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="R4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="S4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="T4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="U4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="V4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="W4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="X4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="Y4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="Z4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="AA4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="AB4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="AC4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="AD4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="AE4" s="9" t="inlineStr">
-        <is>
-          <t>Time of Arrival</t>
-        </is>
-      </c>
-      <c r="AF4" s="8" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="AG4" s="9" t="inlineStr">
+      <c r="A4" s="8" t="n"/>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="C4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="F4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="H4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="I4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="J4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="K4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="L4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="M4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="N4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="O4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="P4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="Q4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="R4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="S4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="T4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="U4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="V4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="W4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="X4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="Y4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="Z4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AA4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AB4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AC4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AD4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AE4" s="10" t="inlineStr">
+        <is>
+          <t>Time of Arrival</t>
+        </is>
+      </c>
+      <c r="AF4" s="9" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="AG4" s="10" t="inlineStr">
         <is>
           <t>Time of Arrival</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="5">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>Oak Lawn</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="6">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="A6" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="7">
-      <c r="A7" s="7" t="n"/>
+      <c r="A7" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="A8" s="11" t="inlineStr">
         <is>
           <t>Hoffman Est.</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="9">
-      <c r="A9" s="11" t="inlineStr">
+      <c r="A9" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="10">
-      <c r="A10" s="7" t="n"/>
+      <c r="A10" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
-      <c r="A11" s="10" t="inlineStr">
+      <c r="A11" s="11" t="inlineStr">
         <is>
           <t>Aurora</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="12">
-      <c r="A12" s="11" t="inlineStr">
+      <c r="A12" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="13">
-      <c r="A13" s="7" t="n"/>
+      <c r="A13" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
-      <c r="A14" s="10" t="inlineStr">
+      <c r="A14" s="11" t="inlineStr">
         <is>
           <t>Kankakee</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="15">
-      <c r="A15" s="11" t="inlineStr">
+      <c r="A15" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="16">
-      <c r="A16" s="7" t="n"/>
+      <c r="A16" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
-      <c r="A17" s="10" t="inlineStr">
+      <c r="A17" s="11" t="inlineStr">
         <is>
           <t>LaSalle</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="18">
-      <c r="A18" s="11" t="inlineStr">
+      <c r="A18" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="19">
-      <c r="A19" s="7" t="n"/>
+      <c r="A19" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
-      <c r="A20" s="10" t="inlineStr">
+      <c r="A20" s="11" t="inlineStr">
         <is>
           <t>Joliet</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="21">
-      <c r="A21" s="11" t="inlineStr">
+      <c r="A21" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="22">
-      <c r="A22" s="7" t="n"/>
+      <c r="A22" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
-      <c r="A23" s="10" t="inlineStr">
+      <c r="A23" s="11" t="inlineStr">
         <is>
           <t>Jesse Brown</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="24">
-      <c r="A24" s="11" t="inlineStr">
+      <c r="A24" s="12" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="10" r="25">
-      <c r="A25" s="7" t="n"/>
+      <c r="A25" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
-      <c r="A26" s="10" t="inlineStr">
+      <c r="A26" s="11" t="inlineStr">
         <is>
           <t>Crown Point</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="21" r="27">
-      <c r="A27" s="6" t="inlineStr">
+      <c r="A27" s="7" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>

</xml_diff>

<commit_message>
with tech/toa borders working
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -58,7 +58,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -144,6 +144,25 @@
       </top>
       <bottom style="thick">
         <color rgb="00001C54"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="00000000"/>
       </bottom>
     </border>
     <border>
@@ -207,8 +226,8 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -216,8 +235,8 @@
     <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>

</xml_diff>

<commit_message>
all signature/initials borders working! just need to account for weekends and holidays
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -58,7 +58,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -166,6 +166,74 @@
       </bottom>
     </border>
     <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+      <bottom style="thick">
+        <color rgb="00001C54"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="00001C54"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="00001C54"/>
+      </right>
+    </border>
+    <border>
       <top style="thick">
         <color rgb="00001C54"/>
       </top>
@@ -221,13 +289,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -240,7 +308,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="16" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -1007,16 +1083,106 @@
           <t>Oak Lawn</t>
         </is>
       </c>
+      <c r="B5" s="12" t="n"/>
+      <c r="C5" s="13" t="n"/>
+      <c r="D5" s="12" t="n"/>
+      <c r="E5" s="13" t="n"/>
+      <c r="F5" s="12" t="n"/>
+      <c r="G5" s="13" t="n"/>
+      <c r="H5" s="12" t="n"/>
+      <c r="I5" s="13" t="n"/>
+      <c r="J5" s="12" t="n"/>
+      <c r="K5" s="13" t="n"/>
+      <c r="L5" s="12" t="n"/>
+      <c r="M5" s="13" t="n"/>
+      <c r="N5" s="12" t="n"/>
+      <c r="O5" s="13" t="n"/>
+      <c r="P5" s="12" t="n"/>
+      <c r="Q5" s="13" t="n"/>
+      <c r="R5" s="12" t="n"/>
+      <c r="S5" s="13" t="n"/>
+      <c r="T5" s="12" t="n"/>
+      <c r="U5" s="13" t="n"/>
+      <c r="V5" s="12" t="n"/>
+      <c r="W5" s="13" t="n"/>
+      <c r="X5" s="12" t="n"/>
+      <c r="Y5" s="13" t="n"/>
+      <c r="Z5" s="12" t="n"/>
+      <c r="AA5" s="13" t="n"/>
+      <c r="AB5" s="12" t="n"/>
+      <c r="AC5" s="13" t="n"/>
+      <c r="AD5" s="12" t="n"/>
+      <c r="AE5" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B6" s="15" t="n"/>
+      <c r="C6" s="16" t="n"/>
+      <c r="D6" s="15" t="n"/>
+      <c r="E6" s="16" t="n"/>
+      <c r="F6" s="15" t="n"/>
+      <c r="G6" s="16" t="n"/>
+      <c r="H6" s="15" t="n"/>
+      <c r="I6" s="16" t="n"/>
+      <c r="J6" s="15" t="n"/>
+      <c r="K6" s="16" t="n"/>
+      <c r="L6" s="15" t="n"/>
+      <c r="M6" s="16" t="n"/>
+      <c r="N6" s="15" t="n"/>
+      <c r="O6" s="16" t="n"/>
+      <c r="P6" s="15" t="n"/>
+      <c r="Q6" s="16" t="n"/>
+      <c r="R6" s="15" t="n"/>
+      <c r="S6" s="16" t="n"/>
+      <c r="T6" s="15" t="n"/>
+      <c r="U6" s="16" t="n"/>
+      <c r="V6" s="15" t="n"/>
+      <c r="W6" s="16" t="n"/>
+      <c r="X6" s="15" t="n"/>
+      <c r="Y6" s="16" t="n"/>
+      <c r="Z6" s="15" t="n"/>
+      <c r="AA6" s="16" t="n"/>
+      <c r="AB6" s="15" t="n"/>
+      <c r="AC6" s="16" t="n"/>
+      <c r="AD6" s="15" t="n"/>
+      <c r="AE6" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="7">
       <c r="A7" s="8" t="n"/>
+      <c r="B7" s="17" t="n"/>
+      <c r="C7" s="18" t="n"/>
+      <c r="D7" s="17" t="n"/>
+      <c r="E7" s="18" t="n"/>
+      <c r="F7" s="17" t="n"/>
+      <c r="G7" s="18" t="n"/>
+      <c r="H7" s="17" t="n"/>
+      <c r="I7" s="18" t="n"/>
+      <c r="J7" s="17" t="n"/>
+      <c r="K7" s="18" t="n"/>
+      <c r="L7" s="17" t="n"/>
+      <c r="M7" s="18" t="n"/>
+      <c r="N7" s="17" t="n"/>
+      <c r="O7" s="18" t="n"/>
+      <c r="P7" s="17" t="n"/>
+      <c r="Q7" s="18" t="n"/>
+      <c r="R7" s="17" t="n"/>
+      <c r="S7" s="18" t="n"/>
+      <c r="T7" s="17" t="n"/>
+      <c r="U7" s="18" t="n"/>
+      <c r="V7" s="17" t="n"/>
+      <c r="W7" s="18" t="n"/>
+      <c r="X7" s="17" t="n"/>
+      <c r="Y7" s="18" t="n"/>
+      <c r="Z7" s="17" t="n"/>
+      <c r="AA7" s="18" t="n"/>
+      <c r="AB7" s="17" t="n"/>
+      <c r="AC7" s="18" t="n"/>
+      <c r="AD7" s="17" t="n"/>
+      <c r="AE7" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
       <c r="A8" s="11" t="inlineStr">
@@ -1024,16 +1190,106 @@
           <t>Hoffman Est.</t>
         </is>
       </c>
+      <c r="B8" s="12" t="n"/>
+      <c r="C8" s="13" t="n"/>
+      <c r="D8" s="12" t="n"/>
+      <c r="E8" s="13" t="n"/>
+      <c r="F8" s="12" t="n"/>
+      <c r="G8" s="13" t="n"/>
+      <c r="H8" s="12" t="n"/>
+      <c r="I8" s="13" t="n"/>
+      <c r="J8" s="12" t="n"/>
+      <c r="K8" s="13" t="n"/>
+      <c r="L8" s="12" t="n"/>
+      <c r="M8" s="13" t="n"/>
+      <c r="N8" s="12" t="n"/>
+      <c r="O8" s="13" t="n"/>
+      <c r="P8" s="12" t="n"/>
+      <c r="Q8" s="13" t="n"/>
+      <c r="R8" s="12" t="n"/>
+      <c r="S8" s="13" t="n"/>
+      <c r="T8" s="12" t="n"/>
+      <c r="U8" s="13" t="n"/>
+      <c r="V8" s="12" t="n"/>
+      <c r="W8" s="13" t="n"/>
+      <c r="X8" s="12" t="n"/>
+      <c r="Y8" s="13" t="n"/>
+      <c r="Z8" s="12" t="n"/>
+      <c r="AA8" s="13" t="n"/>
+      <c r="AB8" s="12" t="n"/>
+      <c r="AC8" s="13" t="n"/>
+      <c r="AD8" s="12" t="n"/>
+      <c r="AE8" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="9">
-      <c r="A9" s="12" t="inlineStr">
+      <c r="A9" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B9" s="15" t="n"/>
+      <c r="C9" s="16" t="n"/>
+      <c r="D9" s="15" t="n"/>
+      <c r="E9" s="16" t="n"/>
+      <c r="F9" s="15" t="n"/>
+      <c r="G9" s="16" t="n"/>
+      <c r="H9" s="15" t="n"/>
+      <c r="I9" s="16" t="n"/>
+      <c r="J9" s="15" t="n"/>
+      <c r="K9" s="16" t="n"/>
+      <c r="L9" s="15" t="n"/>
+      <c r="M9" s="16" t="n"/>
+      <c r="N9" s="15" t="n"/>
+      <c r="O9" s="16" t="n"/>
+      <c r="P9" s="15" t="n"/>
+      <c r="Q9" s="16" t="n"/>
+      <c r="R9" s="15" t="n"/>
+      <c r="S9" s="16" t="n"/>
+      <c r="T9" s="15" t="n"/>
+      <c r="U9" s="16" t="n"/>
+      <c r="V9" s="15" t="n"/>
+      <c r="W9" s="16" t="n"/>
+      <c r="X9" s="15" t="n"/>
+      <c r="Y9" s="16" t="n"/>
+      <c r="Z9" s="15" t="n"/>
+      <c r="AA9" s="16" t="n"/>
+      <c r="AB9" s="15" t="n"/>
+      <c r="AC9" s="16" t="n"/>
+      <c r="AD9" s="15" t="n"/>
+      <c r="AE9" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="10">
       <c r="A10" s="8" t="n"/>
+      <c r="B10" s="17" t="n"/>
+      <c r="C10" s="18" t="n"/>
+      <c r="D10" s="17" t="n"/>
+      <c r="E10" s="18" t="n"/>
+      <c r="F10" s="17" t="n"/>
+      <c r="G10" s="18" t="n"/>
+      <c r="H10" s="17" t="n"/>
+      <c r="I10" s="18" t="n"/>
+      <c r="J10" s="17" t="n"/>
+      <c r="K10" s="18" t="n"/>
+      <c r="L10" s="17" t="n"/>
+      <c r="M10" s="18" t="n"/>
+      <c r="N10" s="17" t="n"/>
+      <c r="O10" s="18" t="n"/>
+      <c r="P10" s="17" t="n"/>
+      <c r="Q10" s="18" t="n"/>
+      <c r="R10" s="17" t="n"/>
+      <c r="S10" s="18" t="n"/>
+      <c r="T10" s="17" t="n"/>
+      <c r="U10" s="18" t="n"/>
+      <c r="V10" s="17" t="n"/>
+      <c r="W10" s="18" t="n"/>
+      <c r="X10" s="17" t="n"/>
+      <c r="Y10" s="18" t="n"/>
+      <c r="Z10" s="17" t="n"/>
+      <c r="AA10" s="18" t="n"/>
+      <c r="AB10" s="17" t="n"/>
+      <c r="AC10" s="18" t="n"/>
+      <c r="AD10" s="17" t="n"/>
+      <c r="AE10" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
       <c r="A11" s="11" t="inlineStr">
@@ -1041,16 +1297,106 @@
           <t>Aurora</t>
         </is>
       </c>
+      <c r="B11" s="12" t="n"/>
+      <c r="C11" s="13" t="n"/>
+      <c r="D11" s="12" t="n"/>
+      <c r="E11" s="13" t="n"/>
+      <c r="F11" s="12" t="n"/>
+      <c r="G11" s="13" t="n"/>
+      <c r="H11" s="12" t="n"/>
+      <c r="I11" s="13" t="n"/>
+      <c r="J11" s="12" t="n"/>
+      <c r="K11" s="13" t="n"/>
+      <c r="L11" s="12" t="n"/>
+      <c r="M11" s="13" t="n"/>
+      <c r="N11" s="12" t="n"/>
+      <c r="O11" s="13" t="n"/>
+      <c r="P11" s="12" t="n"/>
+      <c r="Q11" s="13" t="n"/>
+      <c r="R11" s="12" t="n"/>
+      <c r="S11" s="13" t="n"/>
+      <c r="T11" s="12" t="n"/>
+      <c r="U11" s="13" t="n"/>
+      <c r="V11" s="12" t="n"/>
+      <c r="W11" s="13" t="n"/>
+      <c r="X11" s="12" t="n"/>
+      <c r="Y11" s="13" t="n"/>
+      <c r="Z11" s="12" t="n"/>
+      <c r="AA11" s="13" t="n"/>
+      <c r="AB11" s="12" t="n"/>
+      <c r="AC11" s="13" t="n"/>
+      <c r="AD11" s="12" t="n"/>
+      <c r="AE11" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="12">
-      <c r="A12" s="12" t="inlineStr">
+      <c r="A12" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B12" s="15" t="n"/>
+      <c r="C12" s="16" t="n"/>
+      <c r="D12" s="15" t="n"/>
+      <c r="E12" s="16" t="n"/>
+      <c r="F12" s="15" t="n"/>
+      <c r="G12" s="16" t="n"/>
+      <c r="H12" s="15" t="n"/>
+      <c r="I12" s="16" t="n"/>
+      <c r="J12" s="15" t="n"/>
+      <c r="K12" s="16" t="n"/>
+      <c r="L12" s="15" t="n"/>
+      <c r="M12" s="16" t="n"/>
+      <c r="N12" s="15" t="n"/>
+      <c r="O12" s="16" t="n"/>
+      <c r="P12" s="15" t="n"/>
+      <c r="Q12" s="16" t="n"/>
+      <c r="R12" s="15" t="n"/>
+      <c r="S12" s="16" t="n"/>
+      <c r="T12" s="15" t="n"/>
+      <c r="U12" s="16" t="n"/>
+      <c r="V12" s="15" t="n"/>
+      <c r="W12" s="16" t="n"/>
+      <c r="X12" s="15" t="n"/>
+      <c r="Y12" s="16" t="n"/>
+      <c r="Z12" s="15" t="n"/>
+      <c r="AA12" s="16" t="n"/>
+      <c r="AB12" s="15" t="n"/>
+      <c r="AC12" s="16" t="n"/>
+      <c r="AD12" s="15" t="n"/>
+      <c r="AE12" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="13">
       <c r="A13" s="8" t="n"/>
+      <c r="B13" s="17" t="n"/>
+      <c r="C13" s="18" t="n"/>
+      <c r="D13" s="17" t="n"/>
+      <c r="E13" s="18" t="n"/>
+      <c r="F13" s="17" t="n"/>
+      <c r="G13" s="18" t="n"/>
+      <c r="H13" s="17" t="n"/>
+      <c r="I13" s="18" t="n"/>
+      <c r="J13" s="17" t="n"/>
+      <c r="K13" s="18" t="n"/>
+      <c r="L13" s="17" t="n"/>
+      <c r="M13" s="18" t="n"/>
+      <c r="N13" s="17" t="n"/>
+      <c r="O13" s="18" t="n"/>
+      <c r="P13" s="17" t="n"/>
+      <c r="Q13" s="18" t="n"/>
+      <c r="R13" s="17" t="n"/>
+      <c r="S13" s="18" t="n"/>
+      <c r="T13" s="17" t="n"/>
+      <c r="U13" s="18" t="n"/>
+      <c r="V13" s="17" t="n"/>
+      <c r="W13" s="18" t="n"/>
+      <c r="X13" s="17" t="n"/>
+      <c r="Y13" s="18" t="n"/>
+      <c r="Z13" s="17" t="n"/>
+      <c r="AA13" s="18" t="n"/>
+      <c r="AB13" s="17" t="n"/>
+      <c r="AC13" s="18" t="n"/>
+      <c r="AD13" s="17" t="n"/>
+      <c r="AE13" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
       <c r="A14" s="11" t="inlineStr">
@@ -1058,16 +1404,106 @@
           <t>Kankakee</t>
         </is>
       </c>
+      <c r="B14" s="12" t="n"/>
+      <c r="C14" s="13" t="n"/>
+      <c r="D14" s="12" t="n"/>
+      <c r="E14" s="13" t="n"/>
+      <c r="F14" s="12" t="n"/>
+      <c r="G14" s="13" t="n"/>
+      <c r="H14" s="12" t="n"/>
+      <c r="I14" s="13" t="n"/>
+      <c r="J14" s="12" t="n"/>
+      <c r="K14" s="13" t="n"/>
+      <c r="L14" s="12" t="n"/>
+      <c r="M14" s="13" t="n"/>
+      <c r="N14" s="12" t="n"/>
+      <c r="O14" s="13" t="n"/>
+      <c r="P14" s="12" t="n"/>
+      <c r="Q14" s="13" t="n"/>
+      <c r="R14" s="12" t="n"/>
+      <c r="S14" s="13" t="n"/>
+      <c r="T14" s="12" t="n"/>
+      <c r="U14" s="13" t="n"/>
+      <c r="V14" s="12" t="n"/>
+      <c r="W14" s="13" t="n"/>
+      <c r="X14" s="12" t="n"/>
+      <c r="Y14" s="13" t="n"/>
+      <c r="Z14" s="12" t="n"/>
+      <c r="AA14" s="13" t="n"/>
+      <c r="AB14" s="12" t="n"/>
+      <c r="AC14" s="13" t="n"/>
+      <c r="AD14" s="12" t="n"/>
+      <c r="AE14" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="15">
-      <c r="A15" s="12" t="inlineStr">
+      <c r="A15" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B15" s="15" t="n"/>
+      <c r="C15" s="16" t="n"/>
+      <c r="D15" s="15" t="n"/>
+      <c r="E15" s="16" t="n"/>
+      <c r="F15" s="15" t="n"/>
+      <c r="G15" s="16" t="n"/>
+      <c r="H15" s="15" t="n"/>
+      <c r="I15" s="16" t="n"/>
+      <c r="J15" s="15" t="n"/>
+      <c r="K15" s="16" t="n"/>
+      <c r="L15" s="15" t="n"/>
+      <c r="M15" s="16" t="n"/>
+      <c r="N15" s="15" t="n"/>
+      <c r="O15" s="16" t="n"/>
+      <c r="P15" s="15" t="n"/>
+      <c r="Q15" s="16" t="n"/>
+      <c r="R15" s="15" t="n"/>
+      <c r="S15" s="16" t="n"/>
+      <c r="T15" s="15" t="n"/>
+      <c r="U15" s="16" t="n"/>
+      <c r="V15" s="15" t="n"/>
+      <c r="W15" s="16" t="n"/>
+      <c r="X15" s="15" t="n"/>
+      <c r="Y15" s="16" t="n"/>
+      <c r="Z15" s="15" t="n"/>
+      <c r="AA15" s="16" t="n"/>
+      <c r="AB15" s="15" t="n"/>
+      <c r="AC15" s="16" t="n"/>
+      <c r="AD15" s="15" t="n"/>
+      <c r="AE15" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="16">
       <c r="A16" s="8" t="n"/>
+      <c r="B16" s="17" t="n"/>
+      <c r="C16" s="18" t="n"/>
+      <c r="D16" s="17" t="n"/>
+      <c r="E16" s="18" t="n"/>
+      <c r="F16" s="17" t="n"/>
+      <c r="G16" s="18" t="n"/>
+      <c r="H16" s="17" t="n"/>
+      <c r="I16" s="18" t="n"/>
+      <c r="J16" s="17" t="n"/>
+      <c r="K16" s="18" t="n"/>
+      <c r="L16" s="17" t="n"/>
+      <c r="M16" s="18" t="n"/>
+      <c r="N16" s="17" t="n"/>
+      <c r="O16" s="18" t="n"/>
+      <c r="P16" s="17" t="n"/>
+      <c r="Q16" s="18" t="n"/>
+      <c r="R16" s="17" t="n"/>
+      <c r="S16" s="18" t="n"/>
+      <c r="T16" s="17" t="n"/>
+      <c r="U16" s="18" t="n"/>
+      <c r="V16" s="17" t="n"/>
+      <c r="W16" s="18" t="n"/>
+      <c r="X16" s="17" t="n"/>
+      <c r="Y16" s="18" t="n"/>
+      <c r="Z16" s="17" t="n"/>
+      <c r="AA16" s="18" t="n"/>
+      <c r="AB16" s="17" t="n"/>
+      <c r="AC16" s="18" t="n"/>
+      <c r="AD16" s="17" t="n"/>
+      <c r="AE16" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
       <c r="A17" s="11" t="inlineStr">
@@ -1075,16 +1511,106 @@
           <t>LaSalle</t>
         </is>
       </c>
+      <c r="B17" s="12" t="n"/>
+      <c r="C17" s="13" t="n"/>
+      <c r="D17" s="12" t="n"/>
+      <c r="E17" s="13" t="n"/>
+      <c r="F17" s="12" t="n"/>
+      <c r="G17" s="13" t="n"/>
+      <c r="H17" s="12" t="n"/>
+      <c r="I17" s="13" t="n"/>
+      <c r="J17" s="12" t="n"/>
+      <c r="K17" s="13" t="n"/>
+      <c r="L17" s="12" t="n"/>
+      <c r="M17" s="13" t="n"/>
+      <c r="N17" s="12" t="n"/>
+      <c r="O17" s="13" t="n"/>
+      <c r="P17" s="12" t="n"/>
+      <c r="Q17" s="13" t="n"/>
+      <c r="R17" s="12" t="n"/>
+      <c r="S17" s="13" t="n"/>
+      <c r="T17" s="12" t="n"/>
+      <c r="U17" s="13" t="n"/>
+      <c r="V17" s="12" t="n"/>
+      <c r="W17" s="13" t="n"/>
+      <c r="X17" s="12" t="n"/>
+      <c r="Y17" s="13" t="n"/>
+      <c r="Z17" s="12" t="n"/>
+      <c r="AA17" s="13" t="n"/>
+      <c r="AB17" s="12" t="n"/>
+      <c r="AC17" s="13" t="n"/>
+      <c r="AD17" s="12" t="n"/>
+      <c r="AE17" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="18">
-      <c r="A18" s="12" t="inlineStr">
+      <c r="A18" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B18" s="15" t="n"/>
+      <c r="C18" s="16" t="n"/>
+      <c r="D18" s="15" t="n"/>
+      <c r="E18" s="16" t="n"/>
+      <c r="F18" s="15" t="n"/>
+      <c r="G18" s="16" t="n"/>
+      <c r="H18" s="15" t="n"/>
+      <c r="I18" s="16" t="n"/>
+      <c r="J18" s="15" t="n"/>
+      <c r="K18" s="16" t="n"/>
+      <c r="L18" s="15" t="n"/>
+      <c r="M18" s="16" t="n"/>
+      <c r="N18" s="15" t="n"/>
+      <c r="O18" s="16" t="n"/>
+      <c r="P18" s="15" t="n"/>
+      <c r="Q18" s="16" t="n"/>
+      <c r="R18" s="15" t="n"/>
+      <c r="S18" s="16" t="n"/>
+      <c r="T18" s="15" t="n"/>
+      <c r="U18" s="16" t="n"/>
+      <c r="V18" s="15" t="n"/>
+      <c r="W18" s="16" t="n"/>
+      <c r="X18" s="15" t="n"/>
+      <c r="Y18" s="16" t="n"/>
+      <c r="Z18" s="15" t="n"/>
+      <c r="AA18" s="16" t="n"/>
+      <c r="AB18" s="15" t="n"/>
+      <c r="AC18" s="16" t="n"/>
+      <c r="AD18" s="15" t="n"/>
+      <c r="AE18" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="19">
       <c r="A19" s="8" t="n"/>
+      <c r="B19" s="17" t="n"/>
+      <c r="C19" s="18" t="n"/>
+      <c r="D19" s="17" t="n"/>
+      <c r="E19" s="18" t="n"/>
+      <c r="F19" s="17" t="n"/>
+      <c r="G19" s="18" t="n"/>
+      <c r="H19" s="17" t="n"/>
+      <c r="I19" s="18" t="n"/>
+      <c r="J19" s="17" t="n"/>
+      <c r="K19" s="18" t="n"/>
+      <c r="L19" s="17" t="n"/>
+      <c r="M19" s="18" t="n"/>
+      <c r="N19" s="17" t="n"/>
+      <c r="O19" s="18" t="n"/>
+      <c r="P19" s="17" t="n"/>
+      <c r="Q19" s="18" t="n"/>
+      <c r="R19" s="17" t="n"/>
+      <c r="S19" s="18" t="n"/>
+      <c r="T19" s="17" t="n"/>
+      <c r="U19" s="18" t="n"/>
+      <c r="V19" s="17" t="n"/>
+      <c r="W19" s="18" t="n"/>
+      <c r="X19" s="17" t="n"/>
+      <c r="Y19" s="18" t="n"/>
+      <c r="Z19" s="17" t="n"/>
+      <c r="AA19" s="18" t="n"/>
+      <c r="AB19" s="17" t="n"/>
+      <c r="AC19" s="18" t="n"/>
+      <c r="AD19" s="17" t="n"/>
+      <c r="AE19" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
       <c r="A20" s="11" t="inlineStr">
@@ -1092,16 +1618,106 @@
           <t>Joliet</t>
         </is>
       </c>
+      <c r="B20" s="12" t="n"/>
+      <c r="C20" s="13" t="n"/>
+      <c r="D20" s="12" t="n"/>
+      <c r="E20" s="13" t="n"/>
+      <c r="F20" s="12" t="n"/>
+      <c r="G20" s="13" t="n"/>
+      <c r="H20" s="12" t="n"/>
+      <c r="I20" s="13" t="n"/>
+      <c r="J20" s="12" t="n"/>
+      <c r="K20" s="13" t="n"/>
+      <c r="L20" s="12" t="n"/>
+      <c r="M20" s="13" t="n"/>
+      <c r="N20" s="12" t="n"/>
+      <c r="O20" s="13" t="n"/>
+      <c r="P20" s="12" t="n"/>
+      <c r="Q20" s="13" t="n"/>
+      <c r="R20" s="12" t="n"/>
+      <c r="S20" s="13" t="n"/>
+      <c r="T20" s="12" t="n"/>
+      <c r="U20" s="13" t="n"/>
+      <c r="V20" s="12" t="n"/>
+      <c r="W20" s="13" t="n"/>
+      <c r="X20" s="12" t="n"/>
+      <c r="Y20" s="13" t="n"/>
+      <c r="Z20" s="12" t="n"/>
+      <c r="AA20" s="13" t="n"/>
+      <c r="AB20" s="12" t="n"/>
+      <c r="AC20" s="13" t="n"/>
+      <c r="AD20" s="12" t="n"/>
+      <c r="AE20" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="21">
-      <c r="A21" s="12" t="inlineStr">
+      <c r="A21" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B21" s="15" t="n"/>
+      <c r="C21" s="16" t="n"/>
+      <c r="D21" s="15" t="n"/>
+      <c r="E21" s="16" t="n"/>
+      <c r="F21" s="15" t="n"/>
+      <c r="G21" s="16" t="n"/>
+      <c r="H21" s="15" t="n"/>
+      <c r="I21" s="16" t="n"/>
+      <c r="J21" s="15" t="n"/>
+      <c r="K21" s="16" t="n"/>
+      <c r="L21" s="15" t="n"/>
+      <c r="M21" s="16" t="n"/>
+      <c r="N21" s="15" t="n"/>
+      <c r="O21" s="16" t="n"/>
+      <c r="P21" s="15" t="n"/>
+      <c r="Q21" s="16" t="n"/>
+      <c r="R21" s="15" t="n"/>
+      <c r="S21" s="16" t="n"/>
+      <c r="T21" s="15" t="n"/>
+      <c r="U21" s="16" t="n"/>
+      <c r="V21" s="15" t="n"/>
+      <c r="W21" s="16" t="n"/>
+      <c r="X21" s="15" t="n"/>
+      <c r="Y21" s="16" t="n"/>
+      <c r="Z21" s="15" t="n"/>
+      <c r="AA21" s="16" t="n"/>
+      <c r="AB21" s="15" t="n"/>
+      <c r="AC21" s="16" t="n"/>
+      <c r="AD21" s="15" t="n"/>
+      <c r="AE21" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="22">
       <c r="A22" s="8" t="n"/>
+      <c r="B22" s="17" t="n"/>
+      <c r="C22" s="18" t="n"/>
+      <c r="D22" s="17" t="n"/>
+      <c r="E22" s="18" t="n"/>
+      <c r="F22" s="17" t="n"/>
+      <c r="G22" s="18" t="n"/>
+      <c r="H22" s="17" t="n"/>
+      <c r="I22" s="18" t="n"/>
+      <c r="J22" s="17" t="n"/>
+      <c r="K22" s="18" t="n"/>
+      <c r="L22" s="17" t="n"/>
+      <c r="M22" s="18" t="n"/>
+      <c r="N22" s="17" t="n"/>
+      <c r="O22" s="18" t="n"/>
+      <c r="P22" s="17" t="n"/>
+      <c r="Q22" s="18" t="n"/>
+      <c r="R22" s="17" t="n"/>
+      <c r="S22" s="18" t="n"/>
+      <c r="T22" s="17" t="n"/>
+      <c r="U22" s="18" t="n"/>
+      <c r="V22" s="17" t="n"/>
+      <c r="W22" s="18" t="n"/>
+      <c r="X22" s="17" t="n"/>
+      <c r="Y22" s="18" t="n"/>
+      <c r="Z22" s="17" t="n"/>
+      <c r="AA22" s="18" t="n"/>
+      <c r="AB22" s="17" t="n"/>
+      <c r="AC22" s="18" t="n"/>
+      <c r="AD22" s="17" t="n"/>
+      <c r="AE22" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
       <c r="A23" s="11" t="inlineStr">
@@ -1109,16 +1725,106 @@
           <t>Jesse Brown</t>
         </is>
       </c>
+      <c r="B23" s="12" t="n"/>
+      <c r="C23" s="13" t="n"/>
+      <c r="D23" s="12" t="n"/>
+      <c r="E23" s="13" t="n"/>
+      <c r="F23" s="12" t="n"/>
+      <c r="G23" s="13" t="n"/>
+      <c r="H23" s="12" t="n"/>
+      <c r="I23" s="13" t="n"/>
+      <c r="J23" s="12" t="n"/>
+      <c r="K23" s="13" t="n"/>
+      <c r="L23" s="12" t="n"/>
+      <c r="M23" s="13" t="n"/>
+      <c r="N23" s="12" t="n"/>
+      <c r="O23" s="13" t="n"/>
+      <c r="P23" s="12" t="n"/>
+      <c r="Q23" s="13" t="n"/>
+      <c r="R23" s="12" t="n"/>
+      <c r="S23" s="13" t="n"/>
+      <c r="T23" s="12" t="n"/>
+      <c r="U23" s="13" t="n"/>
+      <c r="V23" s="12" t="n"/>
+      <c r="W23" s="13" t="n"/>
+      <c r="X23" s="12" t="n"/>
+      <c r="Y23" s="13" t="n"/>
+      <c r="Z23" s="12" t="n"/>
+      <c r="AA23" s="13" t="n"/>
+      <c r="AB23" s="12" t="n"/>
+      <c r="AC23" s="13" t="n"/>
+      <c r="AD23" s="12" t="n"/>
+      <c r="AE23" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="24">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="A24" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B24" s="15" t="n"/>
+      <c r="C24" s="16" t="n"/>
+      <c r="D24" s="15" t="n"/>
+      <c r="E24" s="16" t="n"/>
+      <c r="F24" s="15" t="n"/>
+      <c r="G24" s="16" t="n"/>
+      <c r="H24" s="15" t="n"/>
+      <c r="I24" s="16" t="n"/>
+      <c r="J24" s="15" t="n"/>
+      <c r="K24" s="16" t="n"/>
+      <c r="L24" s="15" t="n"/>
+      <c r="M24" s="16" t="n"/>
+      <c r="N24" s="15" t="n"/>
+      <c r="O24" s="16" t="n"/>
+      <c r="P24" s="15" t="n"/>
+      <c r="Q24" s="16" t="n"/>
+      <c r="R24" s="15" t="n"/>
+      <c r="S24" s="16" t="n"/>
+      <c r="T24" s="15" t="n"/>
+      <c r="U24" s="16" t="n"/>
+      <c r="V24" s="15" t="n"/>
+      <c r="W24" s="16" t="n"/>
+      <c r="X24" s="15" t="n"/>
+      <c r="Y24" s="16" t="n"/>
+      <c r="Z24" s="15" t="n"/>
+      <c r="AA24" s="16" t="n"/>
+      <c r="AB24" s="15" t="n"/>
+      <c r="AC24" s="16" t="n"/>
+      <c r="AD24" s="15" t="n"/>
+      <c r="AE24" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="25">
       <c r="A25" s="8" t="n"/>
+      <c r="B25" s="17" t="n"/>
+      <c r="C25" s="18" t="n"/>
+      <c r="D25" s="17" t="n"/>
+      <c r="E25" s="18" t="n"/>
+      <c r="F25" s="17" t="n"/>
+      <c r="G25" s="18" t="n"/>
+      <c r="H25" s="17" t="n"/>
+      <c r="I25" s="18" t="n"/>
+      <c r="J25" s="17" t="n"/>
+      <c r="K25" s="18" t="n"/>
+      <c r="L25" s="17" t="n"/>
+      <c r="M25" s="18" t="n"/>
+      <c r="N25" s="17" t="n"/>
+      <c r="O25" s="18" t="n"/>
+      <c r="P25" s="17" t="n"/>
+      <c r="Q25" s="18" t="n"/>
+      <c r="R25" s="17" t="n"/>
+      <c r="S25" s="18" t="n"/>
+      <c r="T25" s="17" t="n"/>
+      <c r="U25" s="18" t="n"/>
+      <c r="V25" s="17" t="n"/>
+      <c r="W25" s="18" t="n"/>
+      <c r="X25" s="17" t="n"/>
+      <c r="Y25" s="18" t="n"/>
+      <c r="Z25" s="17" t="n"/>
+      <c r="AA25" s="18" t="n"/>
+      <c r="AB25" s="17" t="n"/>
+      <c r="AC25" s="18" t="n"/>
+      <c r="AD25" s="17" t="n"/>
+      <c r="AE25" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
       <c r="A26" s="11" t="inlineStr">
@@ -1126,6 +1832,36 @@
           <t>Crown Point</t>
         </is>
       </c>
+      <c r="B26" s="12" t="n"/>
+      <c r="C26" s="13" t="n"/>
+      <c r="D26" s="12" t="n"/>
+      <c r="E26" s="13" t="n"/>
+      <c r="F26" s="12" t="n"/>
+      <c r="G26" s="13" t="n"/>
+      <c r="H26" s="12" t="n"/>
+      <c r="I26" s="13" t="n"/>
+      <c r="J26" s="12" t="n"/>
+      <c r="K26" s="13" t="n"/>
+      <c r="L26" s="12" t="n"/>
+      <c r="M26" s="13" t="n"/>
+      <c r="N26" s="12" t="n"/>
+      <c r="O26" s="13" t="n"/>
+      <c r="P26" s="12" t="n"/>
+      <c r="Q26" s="13" t="n"/>
+      <c r="R26" s="12" t="n"/>
+      <c r="S26" s="13" t="n"/>
+      <c r="T26" s="12" t="n"/>
+      <c r="U26" s="13" t="n"/>
+      <c r="V26" s="12" t="n"/>
+      <c r="W26" s="13" t="n"/>
+      <c r="X26" s="12" t="n"/>
+      <c r="Y26" s="13" t="n"/>
+      <c r="Z26" s="12" t="n"/>
+      <c r="AA26" s="13" t="n"/>
+      <c r="AB26" s="12" t="n"/>
+      <c r="AC26" s="13" t="n"/>
+      <c r="AD26" s="12" t="n"/>
+      <c r="AE26" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -1133,6 +1869,36 @@
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B27" s="19" t="n"/>
+      <c r="C27" s="20" t="n"/>
+      <c r="D27" s="19" t="n"/>
+      <c r="E27" s="20" t="n"/>
+      <c r="F27" s="19" t="n"/>
+      <c r="G27" s="20" t="n"/>
+      <c r="H27" s="19" t="n"/>
+      <c r="I27" s="20" t="n"/>
+      <c r="J27" s="19" t="n"/>
+      <c r="K27" s="20" t="n"/>
+      <c r="L27" s="19" t="n"/>
+      <c r="M27" s="20" t="n"/>
+      <c r="N27" s="19" t="n"/>
+      <c r="O27" s="20" t="n"/>
+      <c r="P27" s="19" t="n"/>
+      <c r="Q27" s="20" t="n"/>
+      <c r="R27" s="19" t="n"/>
+      <c r="S27" s="20" t="n"/>
+      <c r="T27" s="19" t="n"/>
+      <c r="U27" s="20" t="n"/>
+      <c r="V27" s="19" t="n"/>
+      <c r="W27" s="20" t="n"/>
+      <c r="X27" s="19" t="n"/>
+      <c r="Y27" s="20" t="n"/>
+      <c r="Z27" s="19" t="n"/>
+      <c r="AA27" s="20" t="n"/>
+      <c r="AB27" s="19" t="n"/>
+      <c r="AC27" s="20" t="n"/>
+      <c r="AD27" s="19" t="n"/>
+      <c r="AE27" s="20" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -1603,16 +2369,112 @@
           <t>Oak Lawn</t>
         </is>
       </c>
+      <c r="B5" s="12" t="n"/>
+      <c r="C5" s="13" t="n"/>
+      <c r="D5" s="12" t="n"/>
+      <c r="E5" s="13" t="n"/>
+      <c r="F5" s="12" t="n"/>
+      <c r="G5" s="13" t="n"/>
+      <c r="H5" s="12" t="n"/>
+      <c r="I5" s="13" t="n"/>
+      <c r="J5" s="12" t="n"/>
+      <c r="K5" s="13" t="n"/>
+      <c r="L5" s="12" t="n"/>
+      <c r="M5" s="13" t="n"/>
+      <c r="N5" s="12" t="n"/>
+      <c r="O5" s="13" t="n"/>
+      <c r="P5" s="12" t="n"/>
+      <c r="Q5" s="13" t="n"/>
+      <c r="R5" s="12" t="n"/>
+      <c r="S5" s="13" t="n"/>
+      <c r="T5" s="12" t="n"/>
+      <c r="U5" s="13" t="n"/>
+      <c r="V5" s="12" t="n"/>
+      <c r="W5" s="13" t="n"/>
+      <c r="X5" s="12" t="n"/>
+      <c r="Y5" s="13" t="n"/>
+      <c r="Z5" s="12" t="n"/>
+      <c r="AA5" s="13" t="n"/>
+      <c r="AB5" s="12" t="n"/>
+      <c r="AC5" s="13" t="n"/>
+      <c r="AD5" s="12" t="n"/>
+      <c r="AE5" s="13" t="n"/>
+      <c r="AF5" s="12" t="n"/>
+      <c r="AG5" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B6" s="15" t="n"/>
+      <c r="C6" s="16" t="n"/>
+      <c r="D6" s="15" t="n"/>
+      <c r="E6" s="16" t="n"/>
+      <c r="F6" s="15" t="n"/>
+      <c r="G6" s="16" t="n"/>
+      <c r="H6" s="15" t="n"/>
+      <c r="I6" s="16" t="n"/>
+      <c r="J6" s="15" t="n"/>
+      <c r="K6" s="16" t="n"/>
+      <c r="L6" s="15" t="n"/>
+      <c r="M6" s="16" t="n"/>
+      <c r="N6" s="15" t="n"/>
+      <c r="O6" s="16" t="n"/>
+      <c r="P6" s="15" t="n"/>
+      <c r="Q6" s="16" t="n"/>
+      <c r="R6" s="15" t="n"/>
+      <c r="S6" s="16" t="n"/>
+      <c r="T6" s="15" t="n"/>
+      <c r="U6" s="16" t="n"/>
+      <c r="V6" s="15" t="n"/>
+      <c r="W6" s="16" t="n"/>
+      <c r="X6" s="15" t="n"/>
+      <c r="Y6" s="16" t="n"/>
+      <c r="Z6" s="15" t="n"/>
+      <c r="AA6" s="16" t="n"/>
+      <c r="AB6" s="15" t="n"/>
+      <c r="AC6" s="16" t="n"/>
+      <c r="AD6" s="15" t="n"/>
+      <c r="AE6" s="16" t="n"/>
+      <c r="AF6" s="15" t="n"/>
+      <c r="AG6" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="7">
       <c r="A7" s="8" t="n"/>
+      <c r="B7" s="17" t="n"/>
+      <c r="C7" s="18" t="n"/>
+      <c r="D7" s="17" t="n"/>
+      <c r="E7" s="18" t="n"/>
+      <c r="F7" s="17" t="n"/>
+      <c r="G7" s="18" t="n"/>
+      <c r="H7" s="17" t="n"/>
+      <c r="I7" s="18" t="n"/>
+      <c r="J7" s="17" t="n"/>
+      <c r="K7" s="18" t="n"/>
+      <c r="L7" s="17" t="n"/>
+      <c r="M7" s="18" t="n"/>
+      <c r="N7" s="17" t="n"/>
+      <c r="O7" s="18" t="n"/>
+      <c r="P7" s="17" t="n"/>
+      <c r="Q7" s="18" t="n"/>
+      <c r="R7" s="17" t="n"/>
+      <c r="S7" s="18" t="n"/>
+      <c r="T7" s="17" t="n"/>
+      <c r="U7" s="18" t="n"/>
+      <c r="V7" s="17" t="n"/>
+      <c r="W7" s="18" t="n"/>
+      <c r="X7" s="17" t="n"/>
+      <c r="Y7" s="18" t="n"/>
+      <c r="Z7" s="17" t="n"/>
+      <c r="AA7" s="18" t="n"/>
+      <c r="AB7" s="17" t="n"/>
+      <c r="AC7" s="18" t="n"/>
+      <c r="AD7" s="17" t="n"/>
+      <c r="AE7" s="18" t="n"/>
+      <c r="AF7" s="17" t="n"/>
+      <c r="AG7" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
       <c r="A8" s="11" t="inlineStr">
@@ -1620,16 +2482,112 @@
           <t>Hoffman Est.</t>
         </is>
       </c>
+      <c r="B8" s="12" t="n"/>
+      <c r="C8" s="13" t="n"/>
+      <c r="D8" s="12" t="n"/>
+      <c r="E8" s="13" t="n"/>
+      <c r="F8" s="12" t="n"/>
+      <c r="G8" s="13" t="n"/>
+      <c r="H8" s="12" t="n"/>
+      <c r="I8" s="13" t="n"/>
+      <c r="J8" s="12" t="n"/>
+      <c r="K8" s="13" t="n"/>
+      <c r="L8" s="12" t="n"/>
+      <c r="M8" s="13" t="n"/>
+      <c r="N8" s="12" t="n"/>
+      <c r="O8" s="13" t="n"/>
+      <c r="P8" s="12" t="n"/>
+      <c r="Q8" s="13" t="n"/>
+      <c r="R8" s="12" t="n"/>
+      <c r="S8" s="13" t="n"/>
+      <c r="T8" s="12" t="n"/>
+      <c r="U8" s="13" t="n"/>
+      <c r="V8" s="12" t="n"/>
+      <c r="W8" s="13" t="n"/>
+      <c r="X8" s="12" t="n"/>
+      <c r="Y8" s="13" t="n"/>
+      <c r="Z8" s="12" t="n"/>
+      <c r="AA8" s="13" t="n"/>
+      <c r="AB8" s="12" t="n"/>
+      <c r="AC8" s="13" t="n"/>
+      <c r="AD8" s="12" t="n"/>
+      <c r="AE8" s="13" t="n"/>
+      <c r="AF8" s="12" t="n"/>
+      <c r="AG8" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="9">
-      <c r="A9" s="12" t="inlineStr">
+      <c r="A9" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B9" s="15" t="n"/>
+      <c r="C9" s="16" t="n"/>
+      <c r="D9" s="15" t="n"/>
+      <c r="E9" s="16" t="n"/>
+      <c r="F9" s="15" t="n"/>
+      <c r="G9" s="16" t="n"/>
+      <c r="H9" s="15" t="n"/>
+      <c r="I9" s="16" t="n"/>
+      <c r="J9" s="15" t="n"/>
+      <c r="K9" s="16" t="n"/>
+      <c r="L9" s="15" t="n"/>
+      <c r="M9" s="16" t="n"/>
+      <c r="N9" s="15" t="n"/>
+      <c r="O9" s="16" t="n"/>
+      <c r="P9" s="15" t="n"/>
+      <c r="Q9" s="16" t="n"/>
+      <c r="R9" s="15" t="n"/>
+      <c r="S9" s="16" t="n"/>
+      <c r="T9" s="15" t="n"/>
+      <c r="U9" s="16" t="n"/>
+      <c r="V9" s="15" t="n"/>
+      <c r="W9" s="16" t="n"/>
+      <c r="X9" s="15" t="n"/>
+      <c r="Y9" s="16" t="n"/>
+      <c r="Z9" s="15" t="n"/>
+      <c r="AA9" s="16" t="n"/>
+      <c r="AB9" s="15" t="n"/>
+      <c r="AC9" s="16" t="n"/>
+      <c r="AD9" s="15" t="n"/>
+      <c r="AE9" s="16" t="n"/>
+      <c r="AF9" s="15" t="n"/>
+      <c r="AG9" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="10">
       <c r="A10" s="8" t="n"/>
+      <c r="B10" s="17" t="n"/>
+      <c r="C10" s="18" t="n"/>
+      <c r="D10" s="17" t="n"/>
+      <c r="E10" s="18" t="n"/>
+      <c r="F10" s="17" t="n"/>
+      <c r="G10" s="18" t="n"/>
+      <c r="H10" s="17" t="n"/>
+      <c r="I10" s="18" t="n"/>
+      <c r="J10" s="17" t="n"/>
+      <c r="K10" s="18" t="n"/>
+      <c r="L10" s="17" t="n"/>
+      <c r="M10" s="18" t="n"/>
+      <c r="N10" s="17" t="n"/>
+      <c r="O10" s="18" t="n"/>
+      <c r="P10" s="17" t="n"/>
+      <c r="Q10" s="18" t="n"/>
+      <c r="R10" s="17" t="n"/>
+      <c r="S10" s="18" t="n"/>
+      <c r="T10" s="17" t="n"/>
+      <c r="U10" s="18" t="n"/>
+      <c r="V10" s="17" t="n"/>
+      <c r="W10" s="18" t="n"/>
+      <c r="X10" s="17" t="n"/>
+      <c r="Y10" s="18" t="n"/>
+      <c r="Z10" s="17" t="n"/>
+      <c r="AA10" s="18" t="n"/>
+      <c r="AB10" s="17" t="n"/>
+      <c r="AC10" s="18" t="n"/>
+      <c r="AD10" s="17" t="n"/>
+      <c r="AE10" s="18" t="n"/>
+      <c r="AF10" s="17" t="n"/>
+      <c r="AG10" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
       <c r="A11" s="11" t="inlineStr">
@@ -1637,16 +2595,112 @@
           <t>Aurora</t>
         </is>
       </c>
+      <c r="B11" s="12" t="n"/>
+      <c r="C11" s="13" t="n"/>
+      <c r="D11" s="12" t="n"/>
+      <c r="E11" s="13" t="n"/>
+      <c r="F11" s="12" t="n"/>
+      <c r="G11" s="13" t="n"/>
+      <c r="H11" s="12" t="n"/>
+      <c r="I11" s="13" t="n"/>
+      <c r="J11" s="12" t="n"/>
+      <c r="K11" s="13" t="n"/>
+      <c r="L11" s="12" t="n"/>
+      <c r="M11" s="13" t="n"/>
+      <c r="N11" s="12" t="n"/>
+      <c r="O11" s="13" t="n"/>
+      <c r="P11" s="12" t="n"/>
+      <c r="Q11" s="13" t="n"/>
+      <c r="R11" s="12" t="n"/>
+      <c r="S11" s="13" t="n"/>
+      <c r="T11" s="12" t="n"/>
+      <c r="U11" s="13" t="n"/>
+      <c r="V11" s="12" t="n"/>
+      <c r="W11" s="13" t="n"/>
+      <c r="X11" s="12" t="n"/>
+      <c r="Y11" s="13" t="n"/>
+      <c r="Z11" s="12" t="n"/>
+      <c r="AA11" s="13" t="n"/>
+      <c r="AB11" s="12" t="n"/>
+      <c r="AC11" s="13" t="n"/>
+      <c r="AD11" s="12" t="n"/>
+      <c r="AE11" s="13" t="n"/>
+      <c r="AF11" s="12" t="n"/>
+      <c r="AG11" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="12">
-      <c r="A12" s="12" t="inlineStr">
+      <c r="A12" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B12" s="15" t="n"/>
+      <c r="C12" s="16" t="n"/>
+      <c r="D12" s="15" t="n"/>
+      <c r="E12" s="16" t="n"/>
+      <c r="F12" s="15" t="n"/>
+      <c r="G12" s="16" t="n"/>
+      <c r="H12" s="15" t="n"/>
+      <c r="I12" s="16" t="n"/>
+      <c r="J12" s="15" t="n"/>
+      <c r="K12" s="16" t="n"/>
+      <c r="L12" s="15" t="n"/>
+      <c r="M12" s="16" t="n"/>
+      <c r="N12" s="15" t="n"/>
+      <c r="O12" s="16" t="n"/>
+      <c r="P12" s="15" t="n"/>
+      <c r="Q12" s="16" t="n"/>
+      <c r="R12" s="15" t="n"/>
+      <c r="S12" s="16" t="n"/>
+      <c r="T12" s="15" t="n"/>
+      <c r="U12" s="16" t="n"/>
+      <c r="V12" s="15" t="n"/>
+      <c r="W12" s="16" t="n"/>
+      <c r="X12" s="15" t="n"/>
+      <c r="Y12" s="16" t="n"/>
+      <c r="Z12" s="15" t="n"/>
+      <c r="AA12" s="16" t="n"/>
+      <c r="AB12" s="15" t="n"/>
+      <c r="AC12" s="16" t="n"/>
+      <c r="AD12" s="15" t="n"/>
+      <c r="AE12" s="16" t="n"/>
+      <c r="AF12" s="15" t="n"/>
+      <c r="AG12" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="13">
       <c r="A13" s="8" t="n"/>
+      <c r="B13" s="17" t="n"/>
+      <c r="C13" s="18" t="n"/>
+      <c r="D13" s="17" t="n"/>
+      <c r="E13" s="18" t="n"/>
+      <c r="F13" s="17" t="n"/>
+      <c r="G13" s="18" t="n"/>
+      <c r="H13" s="17" t="n"/>
+      <c r="I13" s="18" t="n"/>
+      <c r="J13" s="17" t="n"/>
+      <c r="K13" s="18" t="n"/>
+      <c r="L13" s="17" t="n"/>
+      <c r="M13" s="18" t="n"/>
+      <c r="N13" s="17" t="n"/>
+      <c r="O13" s="18" t="n"/>
+      <c r="P13" s="17" t="n"/>
+      <c r="Q13" s="18" t="n"/>
+      <c r="R13" s="17" t="n"/>
+      <c r="S13" s="18" t="n"/>
+      <c r="T13" s="17" t="n"/>
+      <c r="U13" s="18" t="n"/>
+      <c r="V13" s="17" t="n"/>
+      <c r="W13" s="18" t="n"/>
+      <c r="X13" s="17" t="n"/>
+      <c r="Y13" s="18" t="n"/>
+      <c r="Z13" s="17" t="n"/>
+      <c r="AA13" s="18" t="n"/>
+      <c r="AB13" s="17" t="n"/>
+      <c r="AC13" s="18" t="n"/>
+      <c r="AD13" s="17" t="n"/>
+      <c r="AE13" s="18" t="n"/>
+      <c r="AF13" s="17" t="n"/>
+      <c r="AG13" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
       <c r="A14" s="11" t="inlineStr">
@@ -1654,16 +2708,112 @@
           <t>Kankakee</t>
         </is>
       </c>
+      <c r="B14" s="12" t="n"/>
+      <c r="C14" s="13" t="n"/>
+      <c r="D14" s="12" t="n"/>
+      <c r="E14" s="13" t="n"/>
+      <c r="F14" s="12" t="n"/>
+      <c r="G14" s="13" t="n"/>
+      <c r="H14" s="12" t="n"/>
+      <c r="I14" s="13" t="n"/>
+      <c r="J14" s="12" t="n"/>
+      <c r="K14" s="13" t="n"/>
+      <c r="L14" s="12" t="n"/>
+      <c r="M14" s="13" t="n"/>
+      <c r="N14" s="12" t="n"/>
+      <c r="O14" s="13" t="n"/>
+      <c r="P14" s="12" t="n"/>
+      <c r="Q14" s="13" t="n"/>
+      <c r="R14" s="12" t="n"/>
+      <c r="S14" s="13" t="n"/>
+      <c r="T14" s="12" t="n"/>
+      <c r="U14" s="13" t="n"/>
+      <c r="V14" s="12" t="n"/>
+      <c r="W14" s="13" t="n"/>
+      <c r="X14" s="12" t="n"/>
+      <c r="Y14" s="13" t="n"/>
+      <c r="Z14" s="12" t="n"/>
+      <c r="AA14" s="13" t="n"/>
+      <c r="AB14" s="12" t="n"/>
+      <c r="AC14" s="13" t="n"/>
+      <c r="AD14" s="12" t="n"/>
+      <c r="AE14" s="13" t="n"/>
+      <c r="AF14" s="12" t="n"/>
+      <c r="AG14" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="15">
-      <c r="A15" s="12" t="inlineStr">
+      <c r="A15" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B15" s="15" t="n"/>
+      <c r="C15" s="16" t="n"/>
+      <c r="D15" s="15" t="n"/>
+      <c r="E15" s="16" t="n"/>
+      <c r="F15" s="15" t="n"/>
+      <c r="G15" s="16" t="n"/>
+      <c r="H15" s="15" t="n"/>
+      <c r="I15" s="16" t="n"/>
+      <c r="J15" s="15" t="n"/>
+      <c r="K15" s="16" t="n"/>
+      <c r="L15" s="15" t="n"/>
+      <c r="M15" s="16" t="n"/>
+      <c r="N15" s="15" t="n"/>
+      <c r="O15" s="16" t="n"/>
+      <c r="P15" s="15" t="n"/>
+      <c r="Q15" s="16" t="n"/>
+      <c r="R15" s="15" t="n"/>
+      <c r="S15" s="16" t="n"/>
+      <c r="T15" s="15" t="n"/>
+      <c r="U15" s="16" t="n"/>
+      <c r="V15" s="15" t="n"/>
+      <c r="W15" s="16" t="n"/>
+      <c r="X15" s="15" t="n"/>
+      <c r="Y15" s="16" t="n"/>
+      <c r="Z15" s="15" t="n"/>
+      <c r="AA15" s="16" t="n"/>
+      <c r="AB15" s="15" t="n"/>
+      <c r="AC15" s="16" t="n"/>
+      <c r="AD15" s="15" t="n"/>
+      <c r="AE15" s="16" t="n"/>
+      <c r="AF15" s="15" t="n"/>
+      <c r="AG15" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="16">
       <c r="A16" s="8" t="n"/>
+      <c r="B16" s="17" t="n"/>
+      <c r="C16" s="18" t="n"/>
+      <c r="D16" s="17" t="n"/>
+      <c r="E16" s="18" t="n"/>
+      <c r="F16" s="17" t="n"/>
+      <c r="G16" s="18" t="n"/>
+      <c r="H16" s="17" t="n"/>
+      <c r="I16" s="18" t="n"/>
+      <c r="J16" s="17" t="n"/>
+      <c r="K16" s="18" t="n"/>
+      <c r="L16" s="17" t="n"/>
+      <c r="M16" s="18" t="n"/>
+      <c r="N16" s="17" t="n"/>
+      <c r="O16" s="18" t="n"/>
+      <c r="P16" s="17" t="n"/>
+      <c r="Q16" s="18" t="n"/>
+      <c r="R16" s="17" t="n"/>
+      <c r="S16" s="18" t="n"/>
+      <c r="T16" s="17" t="n"/>
+      <c r="U16" s="18" t="n"/>
+      <c r="V16" s="17" t="n"/>
+      <c r="W16" s="18" t="n"/>
+      <c r="X16" s="17" t="n"/>
+      <c r="Y16" s="18" t="n"/>
+      <c r="Z16" s="17" t="n"/>
+      <c r="AA16" s="18" t="n"/>
+      <c r="AB16" s="17" t="n"/>
+      <c r="AC16" s="18" t="n"/>
+      <c r="AD16" s="17" t="n"/>
+      <c r="AE16" s="18" t="n"/>
+      <c r="AF16" s="17" t="n"/>
+      <c r="AG16" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
       <c r="A17" s="11" t="inlineStr">
@@ -1671,16 +2821,112 @@
           <t>LaSalle</t>
         </is>
       </c>
+      <c r="B17" s="12" t="n"/>
+      <c r="C17" s="13" t="n"/>
+      <c r="D17" s="12" t="n"/>
+      <c r="E17" s="13" t="n"/>
+      <c r="F17" s="12" t="n"/>
+      <c r="G17" s="13" t="n"/>
+      <c r="H17" s="12" t="n"/>
+      <c r="I17" s="13" t="n"/>
+      <c r="J17" s="12" t="n"/>
+      <c r="K17" s="13" t="n"/>
+      <c r="L17" s="12" t="n"/>
+      <c r="M17" s="13" t="n"/>
+      <c r="N17" s="12" t="n"/>
+      <c r="O17" s="13" t="n"/>
+      <c r="P17" s="12" t="n"/>
+      <c r="Q17" s="13" t="n"/>
+      <c r="R17" s="12" t="n"/>
+      <c r="S17" s="13" t="n"/>
+      <c r="T17" s="12" t="n"/>
+      <c r="U17" s="13" t="n"/>
+      <c r="V17" s="12" t="n"/>
+      <c r="W17" s="13" t="n"/>
+      <c r="X17" s="12" t="n"/>
+      <c r="Y17" s="13" t="n"/>
+      <c r="Z17" s="12" t="n"/>
+      <c r="AA17" s="13" t="n"/>
+      <c r="AB17" s="12" t="n"/>
+      <c r="AC17" s="13" t="n"/>
+      <c r="AD17" s="12" t="n"/>
+      <c r="AE17" s="13" t="n"/>
+      <c r="AF17" s="12" t="n"/>
+      <c r="AG17" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="18">
-      <c r="A18" s="12" t="inlineStr">
+      <c r="A18" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B18" s="15" t="n"/>
+      <c r="C18" s="16" t="n"/>
+      <c r="D18" s="15" t="n"/>
+      <c r="E18" s="16" t="n"/>
+      <c r="F18" s="15" t="n"/>
+      <c r="G18" s="16" t="n"/>
+      <c r="H18" s="15" t="n"/>
+      <c r="I18" s="16" t="n"/>
+      <c r="J18" s="15" t="n"/>
+      <c r="K18" s="16" t="n"/>
+      <c r="L18" s="15" t="n"/>
+      <c r="M18" s="16" t="n"/>
+      <c r="N18" s="15" t="n"/>
+      <c r="O18" s="16" t="n"/>
+      <c r="P18" s="15" t="n"/>
+      <c r="Q18" s="16" t="n"/>
+      <c r="R18" s="15" t="n"/>
+      <c r="S18" s="16" t="n"/>
+      <c r="T18" s="15" t="n"/>
+      <c r="U18" s="16" t="n"/>
+      <c r="V18" s="15" t="n"/>
+      <c r="W18" s="16" t="n"/>
+      <c r="X18" s="15" t="n"/>
+      <c r="Y18" s="16" t="n"/>
+      <c r="Z18" s="15" t="n"/>
+      <c r="AA18" s="16" t="n"/>
+      <c r="AB18" s="15" t="n"/>
+      <c r="AC18" s="16" t="n"/>
+      <c r="AD18" s="15" t="n"/>
+      <c r="AE18" s="16" t="n"/>
+      <c r="AF18" s="15" t="n"/>
+      <c r="AG18" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="19">
       <c r="A19" s="8" t="n"/>
+      <c r="B19" s="17" t="n"/>
+      <c r="C19" s="18" t="n"/>
+      <c r="D19" s="17" t="n"/>
+      <c r="E19" s="18" t="n"/>
+      <c r="F19" s="17" t="n"/>
+      <c r="G19" s="18" t="n"/>
+      <c r="H19" s="17" t="n"/>
+      <c r="I19" s="18" t="n"/>
+      <c r="J19" s="17" t="n"/>
+      <c r="K19" s="18" t="n"/>
+      <c r="L19" s="17" t="n"/>
+      <c r="M19" s="18" t="n"/>
+      <c r="N19" s="17" t="n"/>
+      <c r="O19" s="18" t="n"/>
+      <c r="P19" s="17" t="n"/>
+      <c r="Q19" s="18" t="n"/>
+      <c r="R19" s="17" t="n"/>
+      <c r="S19" s="18" t="n"/>
+      <c r="T19" s="17" t="n"/>
+      <c r="U19" s="18" t="n"/>
+      <c r="V19" s="17" t="n"/>
+      <c r="W19" s="18" t="n"/>
+      <c r="X19" s="17" t="n"/>
+      <c r="Y19" s="18" t="n"/>
+      <c r="Z19" s="17" t="n"/>
+      <c r="AA19" s="18" t="n"/>
+      <c r="AB19" s="17" t="n"/>
+      <c r="AC19" s="18" t="n"/>
+      <c r="AD19" s="17" t="n"/>
+      <c r="AE19" s="18" t="n"/>
+      <c r="AF19" s="17" t="n"/>
+      <c r="AG19" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
       <c r="A20" s="11" t="inlineStr">
@@ -1688,16 +2934,112 @@
           <t>Joliet</t>
         </is>
       </c>
+      <c r="B20" s="12" t="n"/>
+      <c r="C20" s="13" t="n"/>
+      <c r="D20" s="12" t="n"/>
+      <c r="E20" s="13" t="n"/>
+      <c r="F20" s="12" t="n"/>
+      <c r="G20" s="13" t="n"/>
+      <c r="H20" s="12" t="n"/>
+      <c r="I20" s="13" t="n"/>
+      <c r="J20" s="12" t="n"/>
+      <c r="K20" s="13" t="n"/>
+      <c r="L20" s="12" t="n"/>
+      <c r="M20" s="13" t="n"/>
+      <c r="N20" s="12" t="n"/>
+      <c r="O20" s="13" t="n"/>
+      <c r="P20" s="12" t="n"/>
+      <c r="Q20" s="13" t="n"/>
+      <c r="R20" s="12" t="n"/>
+      <c r="S20" s="13" t="n"/>
+      <c r="T20" s="12" t="n"/>
+      <c r="U20" s="13" t="n"/>
+      <c r="V20" s="12" t="n"/>
+      <c r="W20" s="13" t="n"/>
+      <c r="X20" s="12" t="n"/>
+      <c r="Y20" s="13" t="n"/>
+      <c r="Z20" s="12" t="n"/>
+      <c r="AA20" s="13" t="n"/>
+      <c r="AB20" s="12" t="n"/>
+      <c r="AC20" s="13" t="n"/>
+      <c r="AD20" s="12" t="n"/>
+      <c r="AE20" s="13" t="n"/>
+      <c r="AF20" s="12" t="n"/>
+      <c r="AG20" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="21">
-      <c r="A21" s="12" t="inlineStr">
+      <c r="A21" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B21" s="15" t="n"/>
+      <c r="C21" s="16" t="n"/>
+      <c r="D21" s="15" t="n"/>
+      <c r="E21" s="16" t="n"/>
+      <c r="F21" s="15" t="n"/>
+      <c r="G21" s="16" t="n"/>
+      <c r="H21" s="15" t="n"/>
+      <c r="I21" s="16" t="n"/>
+      <c r="J21" s="15" t="n"/>
+      <c r="K21" s="16" t="n"/>
+      <c r="L21" s="15" t="n"/>
+      <c r="M21" s="16" t="n"/>
+      <c r="N21" s="15" t="n"/>
+      <c r="O21" s="16" t="n"/>
+      <c r="P21" s="15" t="n"/>
+      <c r="Q21" s="16" t="n"/>
+      <c r="R21" s="15" t="n"/>
+      <c r="S21" s="16" t="n"/>
+      <c r="T21" s="15" t="n"/>
+      <c r="U21" s="16" t="n"/>
+      <c r="V21" s="15" t="n"/>
+      <c r="W21" s="16" t="n"/>
+      <c r="X21" s="15" t="n"/>
+      <c r="Y21" s="16" t="n"/>
+      <c r="Z21" s="15" t="n"/>
+      <c r="AA21" s="16" t="n"/>
+      <c r="AB21" s="15" t="n"/>
+      <c r="AC21" s="16" t="n"/>
+      <c r="AD21" s="15" t="n"/>
+      <c r="AE21" s="16" t="n"/>
+      <c r="AF21" s="15" t="n"/>
+      <c r="AG21" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="22">
       <c r="A22" s="8" t="n"/>
+      <c r="B22" s="17" t="n"/>
+      <c r="C22" s="18" t="n"/>
+      <c r="D22" s="17" t="n"/>
+      <c r="E22" s="18" t="n"/>
+      <c r="F22" s="17" t="n"/>
+      <c r="G22" s="18" t="n"/>
+      <c r="H22" s="17" t="n"/>
+      <c r="I22" s="18" t="n"/>
+      <c r="J22" s="17" t="n"/>
+      <c r="K22" s="18" t="n"/>
+      <c r="L22" s="17" t="n"/>
+      <c r="M22" s="18" t="n"/>
+      <c r="N22" s="17" t="n"/>
+      <c r="O22" s="18" t="n"/>
+      <c r="P22" s="17" t="n"/>
+      <c r="Q22" s="18" t="n"/>
+      <c r="R22" s="17" t="n"/>
+      <c r="S22" s="18" t="n"/>
+      <c r="T22" s="17" t="n"/>
+      <c r="U22" s="18" t="n"/>
+      <c r="V22" s="17" t="n"/>
+      <c r="W22" s="18" t="n"/>
+      <c r="X22" s="17" t="n"/>
+      <c r="Y22" s="18" t="n"/>
+      <c r="Z22" s="17" t="n"/>
+      <c r="AA22" s="18" t="n"/>
+      <c r="AB22" s="17" t="n"/>
+      <c r="AC22" s="18" t="n"/>
+      <c r="AD22" s="17" t="n"/>
+      <c r="AE22" s="18" t="n"/>
+      <c r="AF22" s="17" t="n"/>
+      <c r="AG22" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
       <c r="A23" s="11" t="inlineStr">
@@ -1705,16 +3047,112 @@
           <t>Jesse Brown</t>
         </is>
       </c>
+      <c r="B23" s="12" t="n"/>
+      <c r="C23" s="13" t="n"/>
+      <c r="D23" s="12" t="n"/>
+      <c r="E23" s="13" t="n"/>
+      <c r="F23" s="12" t="n"/>
+      <c r="G23" s="13" t="n"/>
+      <c r="H23" s="12" t="n"/>
+      <c r="I23" s="13" t="n"/>
+      <c r="J23" s="12" t="n"/>
+      <c r="K23" s="13" t="n"/>
+      <c r="L23" s="12" t="n"/>
+      <c r="M23" s="13" t="n"/>
+      <c r="N23" s="12" t="n"/>
+      <c r="O23" s="13" t="n"/>
+      <c r="P23" s="12" t="n"/>
+      <c r="Q23" s="13" t="n"/>
+      <c r="R23" s="12" t="n"/>
+      <c r="S23" s="13" t="n"/>
+      <c r="T23" s="12" t="n"/>
+      <c r="U23" s="13" t="n"/>
+      <c r="V23" s="12" t="n"/>
+      <c r="W23" s="13" t="n"/>
+      <c r="X23" s="12" t="n"/>
+      <c r="Y23" s="13" t="n"/>
+      <c r="Z23" s="12" t="n"/>
+      <c r="AA23" s="13" t="n"/>
+      <c r="AB23" s="12" t="n"/>
+      <c r="AC23" s="13" t="n"/>
+      <c r="AD23" s="12" t="n"/>
+      <c r="AE23" s="13" t="n"/>
+      <c r="AF23" s="12" t="n"/>
+      <c r="AG23" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="24">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="A24" s="14" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B24" s="15" t="n"/>
+      <c r="C24" s="16" t="n"/>
+      <c r="D24" s="15" t="n"/>
+      <c r="E24" s="16" t="n"/>
+      <c r="F24" s="15" t="n"/>
+      <c r="G24" s="16" t="n"/>
+      <c r="H24" s="15" t="n"/>
+      <c r="I24" s="16" t="n"/>
+      <c r="J24" s="15" t="n"/>
+      <c r="K24" s="16" t="n"/>
+      <c r="L24" s="15" t="n"/>
+      <c r="M24" s="16" t="n"/>
+      <c r="N24" s="15" t="n"/>
+      <c r="O24" s="16" t="n"/>
+      <c r="P24" s="15" t="n"/>
+      <c r="Q24" s="16" t="n"/>
+      <c r="R24" s="15" t="n"/>
+      <c r="S24" s="16" t="n"/>
+      <c r="T24" s="15" t="n"/>
+      <c r="U24" s="16" t="n"/>
+      <c r="V24" s="15" t="n"/>
+      <c r="W24" s="16" t="n"/>
+      <c r="X24" s="15" t="n"/>
+      <c r="Y24" s="16" t="n"/>
+      <c r="Z24" s="15" t="n"/>
+      <c r="AA24" s="16" t="n"/>
+      <c r="AB24" s="15" t="n"/>
+      <c r="AC24" s="16" t="n"/>
+      <c r="AD24" s="15" t="n"/>
+      <c r="AE24" s="16" t="n"/>
+      <c r="AF24" s="15" t="n"/>
+      <c r="AG24" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="10" r="25">
       <c r="A25" s="8" t="n"/>
+      <c r="B25" s="17" t="n"/>
+      <c r="C25" s="18" t="n"/>
+      <c r="D25" s="17" t="n"/>
+      <c r="E25" s="18" t="n"/>
+      <c r="F25" s="17" t="n"/>
+      <c r="G25" s="18" t="n"/>
+      <c r="H25" s="17" t="n"/>
+      <c r="I25" s="18" t="n"/>
+      <c r="J25" s="17" t="n"/>
+      <c r="K25" s="18" t="n"/>
+      <c r="L25" s="17" t="n"/>
+      <c r="M25" s="18" t="n"/>
+      <c r="N25" s="17" t="n"/>
+      <c r="O25" s="18" t="n"/>
+      <c r="P25" s="17" t="n"/>
+      <c r="Q25" s="18" t="n"/>
+      <c r="R25" s="17" t="n"/>
+      <c r="S25" s="18" t="n"/>
+      <c r="T25" s="17" t="n"/>
+      <c r="U25" s="18" t="n"/>
+      <c r="V25" s="17" t="n"/>
+      <c r="W25" s="18" t="n"/>
+      <c r="X25" s="17" t="n"/>
+      <c r="Y25" s="18" t="n"/>
+      <c r="Z25" s="17" t="n"/>
+      <c r="AA25" s="18" t="n"/>
+      <c r="AB25" s="17" t="n"/>
+      <c r="AC25" s="18" t="n"/>
+      <c r="AD25" s="17" t="n"/>
+      <c r="AE25" s="18" t="n"/>
+      <c r="AF25" s="17" t="n"/>
+      <c r="AG25" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
       <c r="A26" s="11" t="inlineStr">
@@ -1722,6 +3160,38 @@
           <t>Crown Point</t>
         </is>
       </c>
+      <c r="B26" s="12" t="n"/>
+      <c r="C26" s="13" t="n"/>
+      <c r="D26" s="12" t="n"/>
+      <c r="E26" s="13" t="n"/>
+      <c r="F26" s="12" t="n"/>
+      <c r="G26" s="13" t="n"/>
+      <c r="H26" s="12" t="n"/>
+      <c r="I26" s="13" t="n"/>
+      <c r="J26" s="12" t="n"/>
+      <c r="K26" s="13" t="n"/>
+      <c r="L26" s="12" t="n"/>
+      <c r="M26" s="13" t="n"/>
+      <c r="N26" s="12" t="n"/>
+      <c r="O26" s="13" t="n"/>
+      <c r="P26" s="12" t="n"/>
+      <c r="Q26" s="13" t="n"/>
+      <c r="R26" s="12" t="n"/>
+      <c r="S26" s="13" t="n"/>
+      <c r="T26" s="12" t="n"/>
+      <c r="U26" s="13" t="n"/>
+      <c r="V26" s="12" t="n"/>
+      <c r="W26" s="13" t="n"/>
+      <c r="X26" s="12" t="n"/>
+      <c r="Y26" s="13" t="n"/>
+      <c r="Z26" s="12" t="n"/>
+      <c r="AA26" s="13" t="n"/>
+      <c r="AB26" s="12" t="n"/>
+      <c r="AC26" s="13" t="n"/>
+      <c r="AD26" s="12" t="n"/>
+      <c r="AE26" s="13" t="n"/>
+      <c r="AF26" s="12" t="n"/>
+      <c r="AG26" s="13" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -1729,6 +3199,38 @@
           <t>Frozen</t>
         </is>
       </c>
+      <c r="B27" s="19" t="n"/>
+      <c r="C27" s="20" t="n"/>
+      <c r="D27" s="19" t="n"/>
+      <c r="E27" s="20" t="n"/>
+      <c r="F27" s="19" t="n"/>
+      <c r="G27" s="20" t="n"/>
+      <c r="H27" s="19" t="n"/>
+      <c r="I27" s="20" t="n"/>
+      <c r="J27" s="19" t="n"/>
+      <c r="K27" s="20" t="n"/>
+      <c r="L27" s="19" t="n"/>
+      <c r="M27" s="20" t="n"/>
+      <c r="N27" s="19" t="n"/>
+      <c r="O27" s="20" t="n"/>
+      <c r="P27" s="19" t="n"/>
+      <c r="Q27" s="20" t="n"/>
+      <c r="R27" s="19" t="n"/>
+      <c r="S27" s="20" t="n"/>
+      <c r="T27" s="19" t="n"/>
+      <c r="U27" s="20" t="n"/>
+      <c r="V27" s="19" t="n"/>
+      <c r="W27" s="20" t="n"/>
+      <c r="X27" s="19" t="n"/>
+      <c r="Y27" s="20" t="n"/>
+      <c r="Z27" s="19" t="n"/>
+      <c r="AA27" s="20" t="n"/>
+      <c r="AB27" s="19" t="n"/>
+      <c r="AC27" s="20" t="n"/>
+      <c r="AD27" s="19" t="n"/>
+      <c r="AE27" s="20" t="n"/>
+      <c r="AF27" s="19" t="n"/>
+      <c r="AG27" s="20" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="33">

</xml_diff>

<commit_message>
with weekends working! just need to add holidays and possibly making a year's worth at once
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -43,6 +43,11 @@
     <font>
       <name val="Calibri"/>
       <sz val="5"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="15"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -297,7 +302,7 @@
   </cellStyleXfs>
   <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -322,21 +327,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="10" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="11" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="8" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="12" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="15" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="16" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="16" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="14" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -1105,10 +1110,26 @@
           <t>Oak Lawn</t>
         </is>
       </c>
-      <c r="B5" s="16" t="n"/>
-      <c r="C5" s="17" t="n"/>
-      <c r="D5" s="16" t="n"/>
-      <c r="E5" s="17" t="n"/>
+      <c r="B5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F5" s="18" t="n"/>
       <c r="G5" s="19" t="n"/>
       <c r="H5" s="18" t="n"/>
@@ -1119,10 +1140,26 @@
       <c r="M5" s="19" t="n"/>
       <c r="N5" s="18" t="n"/>
       <c r="O5" s="19" t="n"/>
-      <c r="P5" s="16" t="n"/>
-      <c r="Q5" s="17" t="n"/>
-      <c r="R5" s="16" t="n"/>
-      <c r="S5" s="17" t="n"/>
+      <c r="P5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T5" s="18" t="n"/>
       <c r="U5" s="19" t="n"/>
       <c r="V5" s="18" t="n"/>
@@ -1133,8 +1170,16 @@
       <c r="AA5" s="19" t="n"/>
       <c r="AB5" s="18" t="n"/>
       <c r="AC5" s="19" t="n"/>
-      <c r="AD5" s="16" t="n"/>
-      <c r="AE5" s="17" t="n"/>
+      <c r="AD5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="6">
       <c r="A6" s="20" t="inlineStr">
@@ -1142,10 +1187,26 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B6" s="21" t="n"/>
-      <c r="C6" s="22" t="n"/>
-      <c r="D6" s="21" t="n"/>
-      <c r="E6" s="22" t="n"/>
+      <c r="B6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F6" s="23" t="n"/>
       <c r="G6" s="24" t="n"/>
       <c r="H6" s="23" t="n"/>
@@ -1156,10 +1217,26 @@
       <c r="M6" s="24" t="n"/>
       <c r="N6" s="23" t="n"/>
       <c r="O6" s="24" t="n"/>
-      <c r="P6" s="21" t="n"/>
-      <c r="Q6" s="22" t="n"/>
-      <c r="R6" s="21" t="n"/>
-      <c r="S6" s="22" t="n"/>
+      <c r="P6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T6" s="23" t="n"/>
       <c r="U6" s="24" t="n"/>
       <c r="V6" s="23" t="n"/>
@@ -1170,8 +1247,16 @@
       <c r="AA6" s="24" t="n"/>
       <c r="AB6" s="23" t="n"/>
       <c r="AC6" s="24" t="n"/>
-      <c r="AD6" s="21" t="n"/>
-      <c r="AE6" s="22" t="n"/>
+      <c r="AD6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="7">
       <c r="A7" s="10" t="n"/>
@@ -1212,10 +1297,26 @@
           <t>Hoffman Est.</t>
         </is>
       </c>
-      <c r="B8" s="16" t="n"/>
-      <c r="C8" s="17" t="n"/>
-      <c r="D8" s="16" t="n"/>
-      <c r="E8" s="17" t="n"/>
+      <c r="B8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F8" s="18" t="n"/>
       <c r="G8" s="19" t="n"/>
       <c r="H8" s="18" t="n"/>
@@ -1226,10 +1327,26 @@
       <c r="M8" s="19" t="n"/>
       <c r="N8" s="18" t="n"/>
       <c r="O8" s="19" t="n"/>
-      <c r="P8" s="16" t="n"/>
-      <c r="Q8" s="17" t="n"/>
-      <c r="R8" s="16" t="n"/>
-      <c r="S8" s="17" t="n"/>
+      <c r="P8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T8" s="18" t="n"/>
       <c r="U8" s="19" t="n"/>
       <c r="V8" s="18" t="n"/>
@@ -1240,8 +1357,16 @@
       <c r="AA8" s="19" t="n"/>
       <c r="AB8" s="18" t="n"/>
       <c r="AC8" s="19" t="n"/>
-      <c r="AD8" s="16" t="n"/>
-      <c r="AE8" s="17" t="n"/>
+      <c r="AD8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="9">
       <c r="A9" s="20" t="inlineStr">
@@ -1249,10 +1374,26 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B9" s="21" t="n"/>
-      <c r="C9" s="22" t="n"/>
-      <c r="D9" s="21" t="n"/>
-      <c r="E9" s="22" t="n"/>
+      <c r="B9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F9" s="23" t="n"/>
       <c r="G9" s="24" t="n"/>
       <c r="H9" s="23" t="n"/>
@@ -1263,10 +1404,26 @@
       <c r="M9" s="24" t="n"/>
       <c r="N9" s="23" t="n"/>
       <c r="O9" s="24" t="n"/>
-      <c r="P9" s="21" t="n"/>
-      <c r="Q9" s="22" t="n"/>
-      <c r="R9" s="21" t="n"/>
-      <c r="S9" s="22" t="n"/>
+      <c r="P9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T9" s="23" t="n"/>
       <c r="U9" s="24" t="n"/>
       <c r="V9" s="23" t="n"/>
@@ -1277,8 +1434,16 @@
       <c r="AA9" s="24" t="n"/>
       <c r="AB9" s="23" t="n"/>
       <c r="AC9" s="24" t="n"/>
-      <c r="AD9" s="21" t="n"/>
-      <c r="AE9" s="22" t="n"/>
+      <c r="AD9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="10">
       <c r="A10" s="10" t="n"/>
@@ -1319,10 +1484,26 @@
           <t>Aurora</t>
         </is>
       </c>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="17" t="n"/>
-      <c r="D11" s="16" t="n"/>
-      <c r="E11" s="17" t="n"/>
+      <c r="B11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F11" s="18" t="n"/>
       <c r="G11" s="19" t="n"/>
       <c r="H11" s="18" t="n"/>
@@ -1333,10 +1514,26 @@
       <c r="M11" s="19" t="n"/>
       <c r="N11" s="18" t="n"/>
       <c r="O11" s="19" t="n"/>
-      <c r="P11" s="16" t="n"/>
-      <c r="Q11" s="17" t="n"/>
-      <c r="R11" s="16" t="n"/>
-      <c r="S11" s="17" t="n"/>
+      <c r="P11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T11" s="18" t="n"/>
       <c r="U11" s="19" t="n"/>
       <c r="V11" s="18" t="n"/>
@@ -1347,8 +1544,16 @@
       <c r="AA11" s="19" t="n"/>
       <c r="AB11" s="18" t="n"/>
       <c r="AC11" s="19" t="n"/>
-      <c r="AD11" s="16" t="n"/>
-      <c r="AE11" s="17" t="n"/>
+      <c r="AD11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="12">
       <c r="A12" s="20" t="inlineStr">
@@ -1356,10 +1561,26 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B12" s="21" t="n"/>
-      <c r="C12" s="22" t="n"/>
-      <c r="D12" s="21" t="n"/>
-      <c r="E12" s="22" t="n"/>
+      <c r="B12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F12" s="23" t="n"/>
       <c r="G12" s="24" t="n"/>
       <c r="H12" s="23" t="n"/>
@@ -1370,10 +1591,26 @@
       <c r="M12" s="24" t="n"/>
       <c r="N12" s="23" t="n"/>
       <c r="O12" s="24" t="n"/>
-      <c r="P12" s="21" t="n"/>
-      <c r="Q12" s="22" t="n"/>
-      <c r="R12" s="21" t="n"/>
-      <c r="S12" s="22" t="n"/>
+      <c r="P12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T12" s="23" t="n"/>
       <c r="U12" s="24" t="n"/>
       <c r="V12" s="23" t="n"/>
@@ -1384,8 +1621,16 @@
       <c r="AA12" s="24" t="n"/>
       <c r="AB12" s="23" t="n"/>
       <c r="AC12" s="24" t="n"/>
-      <c r="AD12" s="21" t="n"/>
-      <c r="AE12" s="22" t="n"/>
+      <c r="AD12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="13">
       <c r="A13" s="10" t="n"/>
@@ -1426,10 +1671,26 @@
           <t>Kankakee</t>
         </is>
       </c>
-      <c r="B14" s="16" t="n"/>
-      <c r="C14" s="17" t="n"/>
-      <c r="D14" s="16" t="n"/>
-      <c r="E14" s="17" t="n"/>
+      <c r="B14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F14" s="18" t="n"/>
       <c r="G14" s="19" t="n"/>
       <c r="H14" s="18" t="n"/>
@@ -1440,10 +1701,26 @@
       <c r="M14" s="19" t="n"/>
       <c r="N14" s="18" t="n"/>
       <c r="O14" s="19" t="n"/>
-      <c r="P14" s="16" t="n"/>
-      <c r="Q14" s="17" t="n"/>
-      <c r="R14" s="16" t="n"/>
-      <c r="S14" s="17" t="n"/>
+      <c r="P14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T14" s="18" t="n"/>
       <c r="U14" s="19" t="n"/>
       <c r="V14" s="18" t="n"/>
@@ -1454,8 +1731,16 @@
       <c r="AA14" s="19" t="n"/>
       <c r="AB14" s="18" t="n"/>
       <c r="AC14" s="19" t="n"/>
-      <c r="AD14" s="16" t="n"/>
-      <c r="AE14" s="17" t="n"/>
+      <c r="AD14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="15">
       <c r="A15" s="20" t="inlineStr">
@@ -1463,10 +1748,26 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B15" s="21" t="n"/>
-      <c r="C15" s="22" t="n"/>
-      <c r="D15" s="21" t="n"/>
-      <c r="E15" s="22" t="n"/>
+      <c r="B15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F15" s="23" t="n"/>
       <c r="G15" s="24" t="n"/>
       <c r="H15" s="23" t="n"/>
@@ -1477,10 +1778,26 @@
       <c r="M15" s="24" t="n"/>
       <c r="N15" s="23" t="n"/>
       <c r="O15" s="24" t="n"/>
-      <c r="P15" s="21" t="n"/>
-      <c r="Q15" s="22" t="n"/>
-      <c r="R15" s="21" t="n"/>
-      <c r="S15" s="22" t="n"/>
+      <c r="P15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T15" s="23" t="n"/>
       <c r="U15" s="24" t="n"/>
       <c r="V15" s="23" t="n"/>
@@ -1491,8 +1808,16 @@
       <c r="AA15" s="24" t="n"/>
       <c r="AB15" s="23" t="n"/>
       <c r="AC15" s="24" t="n"/>
-      <c r="AD15" s="21" t="n"/>
-      <c r="AE15" s="22" t="n"/>
+      <c r="AD15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="16">
       <c r="A16" s="10" t="n"/>
@@ -1533,10 +1858,26 @@
           <t>LaSalle</t>
         </is>
       </c>
-      <c r="B17" s="16" t="n"/>
-      <c r="C17" s="17" t="n"/>
-      <c r="D17" s="16" t="n"/>
-      <c r="E17" s="17" t="n"/>
+      <c r="B17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F17" s="18" t="n"/>
       <c r="G17" s="19" t="n"/>
       <c r="H17" s="18" t="n"/>
@@ -1547,10 +1888,26 @@
       <c r="M17" s="19" t="n"/>
       <c r="N17" s="18" t="n"/>
       <c r="O17" s="19" t="n"/>
-      <c r="P17" s="16" t="n"/>
-      <c r="Q17" s="17" t="n"/>
-      <c r="R17" s="16" t="n"/>
-      <c r="S17" s="17" t="n"/>
+      <c r="P17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T17" s="18" t="n"/>
       <c r="U17" s="19" t="n"/>
       <c r="V17" s="18" t="n"/>
@@ -1561,8 +1918,16 @@
       <c r="AA17" s="19" t="n"/>
       <c r="AB17" s="18" t="n"/>
       <c r="AC17" s="19" t="n"/>
-      <c r="AD17" s="16" t="n"/>
-      <c r="AE17" s="17" t="n"/>
+      <c r="AD17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="18">
       <c r="A18" s="20" t="inlineStr">
@@ -1570,10 +1935,26 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B18" s="21" t="n"/>
-      <c r="C18" s="22" t="n"/>
-      <c r="D18" s="21" t="n"/>
-      <c r="E18" s="22" t="n"/>
+      <c r="B18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F18" s="23" t="n"/>
       <c r="G18" s="24" t="n"/>
       <c r="H18" s="23" t="n"/>
@@ -1584,10 +1965,26 @@
       <c r="M18" s="24" t="n"/>
       <c r="N18" s="23" t="n"/>
       <c r="O18" s="24" t="n"/>
-      <c r="P18" s="21" t="n"/>
-      <c r="Q18" s="22" t="n"/>
-      <c r="R18" s="21" t="n"/>
-      <c r="S18" s="22" t="n"/>
+      <c r="P18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T18" s="23" t="n"/>
       <c r="U18" s="24" t="n"/>
       <c r="V18" s="23" t="n"/>
@@ -1598,8 +1995,16 @@
       <c r="AA18" s="24" t="n"/>
       <c r="AB18" s="23" t="n"/>
       <c r="AC18" s="24" t="n"/>
-      <c r="AD18" s="21" t="n"/>
-      <c r="AE18" s="22" t="n"/>
+      <c r="AD18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="19">
       <c r="A19" s="10" t="n"/>
@@ -1640,10 +2045,26 @@
           <t>Joliet</t>
         </is>
       </c>
-      <c r="B20" s="16" t="n"/>
-      <c r="C20" s="17" t="n"/>
-      <c r="D20" s="16" t="n"/>
-      <c r="E20" s="17" t="n"/>
+      <c r="B20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F20" s="18" t="n"/>
       <c r="G20" s="19" t="n"/>
       <c r="H20" s="18" t="n"/>
@@ -1654,10 +2075,26 @@
       <c r="M20" s="19" t="n"/>
       <c r="N20" s="18" t="n"/>
       <c r="O20" s="19" t="n"/>
-      <c r="P20" s="16" t="n"/>
-      <c r="Q20" s="17" t="n"/>
-      <c r="R20" s="16" t="n"/>
-      <c r="S20" s="17" t="n"/>
+      <c r="P20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T20" s="18" t="n"/>
       <c r="U20" s="19" t="n"/>
       <c r="V20" s="18" t="n"/>
@@ -1668,8 +2105,16 @@
       <c r="AA20" s="19" t="n"/>
       <c r="AB20" s="18" t="n"/>
       <c r="AC20" s="19" t="n"/>
-      <c r="AD20" s="16" t="n"/>
-      <c r="AE20" s="17" t="n"/>
+      <c r="AD20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="21">
       <c r="A21" s="20" t="inlineStr">
@@ -1677,10 +2122,26 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B21" s="21" t="n"/>
-      <c r="C21" s="22" t="n"/>
-      <c r="D21" s="21" t="n"/>
-      <c r="E21" s="22" t="n"/>
+      <c r="B21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F21" s="23" t="n"/>
       <c r="G21" s="24" t="n"/>
       <c r="H21" s="23" t="n"/>
@@ -1691,10 +2152,26 @@
       <c r="M21" s="24" t="n"/>
       <c r="N21" s="23" t="n"/>
       <c r="O21" s="24" t="n"/>
-      <c r="P21" s="21" t="n"/>
-      <c r="Q21" s="22" t="n"/>
-      <c r="R21" s="21" t="n"/>
-      <c r="S21" s="22" t="n"/>
+      <c r="P21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T21" s="23" t="n"/>
       <c r="U21" s="24" t="n"/>
       <c r="V21" s="23" t="n"/>
@@ -1705,8 +2182,16 @@
       <c r="AA21" s="24" t="n"/>
       <c r="AB21" s="23" t="n"/>
       <c r="AC21" s="24" t="n"/>
-      <c r="AD21" s="21" t="n"/>
-      <c r="AE21" s="22" t="n"/>
+      <c r="AD21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="22">
       <c r="A22" s="10" t="n"/>
@@ -1747,10 +2232,26 @@
           <t>Jesse Brown</t>
         </is>
       </c>
-      <c r="B23" s="16" t="n"/>
-      <c r="C23" s="17" t="n"/>
-      <c r="D23" s="16" t="n"/>
-      <c r="E23" s="17" t="n"/>
+      <c r="B23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F23" s="18" t="n"/>
       <c r="G23" s="19" t="n"/>
       <c r="H23" s="18" t="n"/>
@@ -1761,10 +2262,26 @@
       <c r="M23" s="19" t="n"/>
       <c r="N23" s="18" t="n"/>
       <c r="O23" s="19" t="n"/>
-      <c r="P23" s="16" t="n"/>
-      <c r="Q23" s="17" t="n"/>
-      <c r="R23" s="16" t="n"/>
-      <c r="S23" s="17" t="n"/>
+      <c r="P23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T23" s="18" t="n"/>
       <c r="U23" s="19" t="n"/>
       <c r="V23" s="18" t="n"/>
@@ -1775,8 +2292,16 @@
       <c r="AA23" s="19" t="n"/>
       <c r="AB23" s="18" t="n"/>
       <c r="AC23" s="19" t="n"/>
-      <c r="AD23" s="16" t="n"/>
-      <c r="AE23" s="17" t="n"/>
+      <c r="AD23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="24">
       <c r="A24" s="20" t="inlineStr">
@@ -1784,10 +2309,26 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B24" s="21" t="n"/>
-      <c r="C24" s="22" t="n"/>
-      <c r="D24" s="21" t="n"/>
-      <c r="E24" s="22" t="n"/>
+      <c r="B24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F24" s="23" t="n"/>
       <c r="G24" s="24" t="n"/>
       <c r="H24" s="23" t="n"/>
@@ -1798,10 +2339,26 @@
       <c r="M24" s="24" t="n"/>
       <c r="N24" s="23" t="n"/>
       <c r="O24" s="24" t="n"/>
-      <c r="P24" s="21" t="n"/>
-      <c r="Q24" s="22" t="n"/>
-      <c r="R24" s="21" t="n"/>
-      <c r="S24" s="22" t="n"/>
+      <c r="P24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T24" s="23" t="n"/>
       <c r="U24" s="24" t="n"/>
       <c r="V24" s="23" t="n"/>
@@ -1812,8 +2369,16 @@
       <c r="AA24" s="24" t="n"/>
       <c r="AB24" s="23" t="n"/>
       <c r="AC24" s="24" t="n"/>
-      <c r="AD24" s="21" t="n"/>
-      <c r="AE24" s="22" t="n"/>
+      <c r="AD24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="25">
       <c r="A25" s="10" t="n"/>
@@ -1854,10 +2419,26 @@
           <t>Crown Point</t>
         </is>
       </c>
-      <c r="B26" s="16" t="n"/>
-      <c r="C26" s="17" t="n"/>
-      <c r="D26" s="16" t="n"/>
-      <c r="E26" s="17" t="n"/>
+      <c r="B26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F26" s="18" t="n"/>
       <c r="G26" s="19" t="n"/>
       <c r="H26" s="18" t="n"/>
@@ -1868,10 +2449,26 @@
       <c r="M26" s="19" t="n"/>
       <c r="N26" s="18" t="n"/>
       <c r="O26" s="19" t="n"/>
-      <c r="P26" s="16" t="n"/>
-      <c r="Q26" s="17" t="n"/>
-      <c r="R26" s="16" t="n"/>
-      <c r="S26" s="17" t="n"/>
+      <c r="P26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T26" s="18" t="n"/>
       <c r="U26" s="19" t="n"/>
       <c r="V26" s="18" t="n"/>
@@ -1882,8 +2479,16 @@
       <c r="AA26" s="19" t="n"/>
       <c r="AB26" s="18" t="n"/>
       <c r="AC26" s="19" t="n"/>
-      <c r="AD26" s="16" t="n"/>
-      <c r="AE26" s="17" t="n"/>
+      <c r="AD26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="27">
       <c r="A27" s="9" t="inlineStr">
@@ -1891,10 +2496,26 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B27" s="29" t="n"/>
-      <c r="C27" s="30" t="n"/>
-      <c r="D27" s="29" t="n"/>
-      <c r="E27" s="30" t="n"/>
+      <c r="B27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F27" s="31" t="n"/>
       <c r="G27" s="32" t="n"/>
       <c r="H27" s="31" t="n"/>
@@ -1905,10 +2526,26 @@
       <c r="M27" s="32" t="n"/>
       <c r="N27" s="31" t="n"/>
       <c r="O27" s="32" t="n"/>
-      <c r="P27" s="29" t="n"/>
-      <c r="Q27" s="30" t="n"/>
-      <c r="R27" s="29" t="n"/>
-      <c r="S27" s="30" t="n"/>
+      <c r="P27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="T27" s="31" t="n"/>
       <c r="U27" s="32" t="n"/>
       <c r="V27" s="31" t="n"/>
@@ -1919,8 +2556,16 @@
       <c r="AA27" s="32" t="n"/>
       <c r="AB27" s="31" t="n"/>
       <c r="AC27" s="32" t="n"/>
-      <c r="AD27" s="29" t="n"/>
-      <c r="AE27" s="30" t="n"/>
+      <c r="AD27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -2391,8 +3036,16 @@
           <t>Oak Lawn</t>
         </is>
       </c>
-      <c r="B5" s="16" t="n"/>
-      <c r="C5" s="17" t="n"/>
+      <c r="B5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D5" s="18" t="n"/>
       <c r="E5" s="19" t="n"/>
       <c r="F5" s="18" t="n"/>
@@ -2403,10 +3056,26 @@
       <c r="K5" s="19" t="n"/>
       <c r="L5" s="18" t="n"/>
       <c r="M5" s="19" t="n"/>
-      <c r="N5" s="16" t="n"/>
-      <c r="O5" s="17" t="n"/>
-      <c r="P5" s="16" t="n"/>
-      <c r="Q5" s="17" t="n"/>
+      <c r="N5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R5" s="18" t="n"/>
       <c r="S5" s="19" t="n"/>
       <c r="T5" s="18" t="n"/>
@@ -2417,10 +3086,26 @@
       <c r="Y5" s="19" t="n"/>
       <c r="Z5" s="18" t="n"/>
       <c r="AA5" s="19" t="n"/>
-      <c r="AB5" s="16" t="n"/>
-      <c r="AC5" s="17" t="n"/>
-      <c r="AD5" s="16" t="n"/>
-      <c r="AE5" s="17" t="n"/>
+      <c r="AB5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF5" s="18" t="n"/>
       <c r="AG5" s="19" t="n"/>
     </row>
@@ -2430,8 +3115,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B6" s="21" t="n"/>
-      <c r="C6" s="22" t="n"/>
+      <c r="B6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D6" s="23" t="n"/>
       <c r="E6" s="24" t="n"/>
       <c r="F6" s="23" t="n"/>
@@ -2442,10 +3135,26 @@
       <c r="K6" s="24" t="n"/>
       <c r="L6" s="23" t="n"/>
       <c r="M6" s="24" t="n"/>
-      <c r="N6" s="21" t="n"/>
-      <c r="O6" s="22" t="n"/>
-      <c r="P6" s="21" t="n"/>
-      <c r="Q6" s="22" t="n"/>
+      <c r="N6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R6" s="23" t="n"/>
       <c r="S6" s="24" t="n"/>
       <c r="T6" s="23" t="n"/>
@@ -2456,10 +3165,26 @@
       <c r="Y6" s="24" t="n"/>
       <c r="Z6" s="23" t="n"/>
       <c r="AA6" s="24" t="n"/>
-      <c r="AB6" s="21" t="n"/>
-      <c r="AC6" s="22" t="n"/>
-      <c r="AD6" s="21" t="n"/>
-      <c r="AE6" s="22" t="n"/>
+      <c r="AB6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF6" s="23" t="n"/>
       <c r="AG6" s="24" t="n"/>
     </row>
@@ -2504,8 +3229,16 @@
           <t>Hoffman Est.</t>
         </is>
       </c>
-      <c r="B8" s="16" t="n"/>
-      <c r="C8" s="17" t="n"/>
+      <c r="B8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D8" s="18" t="n"/>
       <c r="E8" s="19" t="n"/>
       <c r="F8" s="18" t="n"/>
@@ -2516,10 +3249,26 @@
       <c r="K8" s="19" t="n"/>
       <c r="L8" s="18" t="n"/>
       <c r="M8" s="19" t="n"/>
-      <c r="N8" s="16" t="n"/>
-      <c r="O8" s="17" t="n"/>
-      <c r="P8" s="16" t="n"/>
-      <c r="Q8" s="17" t="n"/>
+      <c r="N8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R8" s="18" t="n"/>
       <c r="S8" s="19" t="n"/>
       <c r="T8" s="18" t="n"/>
@@ -2530,10 +3279,26 @@
       <c r="Y8" s="19" t="n"/>
       <c r="Z8" s="18" t="n"/>
       <c r="AA8" s="19" t="n"/>
-      <c r="AB8" s="16" t="n"/>
-      <c r="AC8" s="17" t="n"/>
-      <c r="AD8" s="16" t="n"/>
-      <c r="AE8" s="17" t="n"/>
+      <c r="AB8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF8" s="18" t="n"/>
       <c r="AG8" s="19" t="n"/>
     </row>
@@ -2543,8 +3308,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B9" s="21" t="n"/>
-      <c r="C9" s="22" t="n"/>
+      <c r="B9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D9" s="23" t="n"/>
       <c r="E9" s="24" t="n"/>
       <c r="F9" s="23" t="n"/>
@@ -2555,10 +3328,26 @@
       <c r="K9" s="24" t="n"/>
       <c r="L9" s="23" t="n"/>
       <c r="M9" s="24" t="n"/>
-      <c r="N9" s="21" t="n"/>
-      <c r="O9" s="22" t="n"/>
-      <c r="P9" s="21" t="n"/>
-      <c r="Q9" s="22" t="n"/>
+      <c r="N9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R9" s="23" t="n"/>
       <c r="S9" s="24" t="n"/>
       <c r="T9" s="23" t="n"/>
@@ -2569,10 +3358,26 @@
       <c r="Y9" s="24" t="n"/>
       <c r="Z9" s="23" t="n"/>
       <c r="AA9" s="24" t="n"/>
-      <c r="AB9" s="21" t="n"/>
-      <c r="AC9" s="22" t="n"/>
-      <c r="AD9" s="21" t="n"/>
-      <c r="AE9" s="22" t="n"/>
+      <c r="AB9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF9" s="23" t="n"/>
       <c r="AG9" s="24" t="n"/>
     </row>
@@ -2617,8 +3422,16 @@
           <t>Aurora</t>
         </is>
       </c>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="17" t="n"/>
+      <c r="B11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D11" s="18" t="n"/>
       <c r="E11" s="19" t="n"/>
       <c r="F11" s="18" t="n"/>
@@ -2629,10 +3442,26 @@
       <c r="K11" s="19" t="n"/>
       <c r="L11" s="18" t="n"/>
       <c r="M11" s="19" t="n"/>
-      <c r="N11" s="16" t="n"/>
-      <c r="O11" s="17" t="n"/>
-      <c r="P11" s="16" t="n"/>
-      <c r="Q11" s="17" t="n"/>
+      <c r="N11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R11" s="18" t="n"/>
       <c r="S11" s="19" t="n"/>
       <c r="T11" s="18" t="n"/>
@@ -2643,10 +3472,26 @@
       <c r="Y11" s="19" t="n"/>
       <c r="Z11" s="18" t="n"/>
       <c r="AA11" s="19" t="n"/>
-      <c r="AB11" s="16" t="n"/>
-      <c r="AC11" s="17" t="n"/>
-      <c r="AD11" s="16" t="n"/>
-      <c r="AE11" s="17" t="n"/>
+      <c r="AB11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF11" s="18" t="n"/>
       <c r="AG11" s="19" t="n"/>
     </row>
@@ -2656,8 +3501,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B12" s="21" t="n"/>
-      <c r="C12" s="22" t="n"/>
+      <c r="B12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D12" s="23" t="n"/>
       <c r="E12" s="24" t="n"/>
       <c r="F12" s="23" t="n"/>
@@ -2668,10 +3521,26 @@
       <c r="K12" s="24" t="n"/>
       <c r="L12" s="23" t="n"/>
       <c r="M12" s="24" t="n"/>
-      <c r="N12" s="21" t="n"/>
-      <c r="O12" s="22" t="n"/>
-      <c r="P12" s="21" t="n"/>
-      <c r="Q12" s="22" t="n"/>
+      <c r="N12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R12" s="23" t="n"/>
       <c r="S12" s="24" t="n"/>
       <c r="T12" s="23" t="n"/>
@@ -2682,10 +3551,26 @@
       <c r="Y12" s="24" t="n"/>
       <c r="Z12" s="23" t="n"/>
       <c r="AA12" s="24" t="n"/>
-      <c r="AB12" s="21" t="n"/>
-      <c r="AC12" s="22" t="n"/>
-      <c r="AD12" s="21" t="n"/>
-      <c r="AE12" s="22" t="n"/>
+      <c r="AB12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF12" s="23" t="n"/>
       <c r="AG12" s="24" t="n"/>
     </row>
@@ -2730,8 +3615,16 @@
           <t>Kankakee</t>
         </is>
       </c>
-      <c r="B14" s="16" t="n"/>
-      <c r="C14" s="17" t="n"/>
+      <c r="B14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D14" s="18" t="n"/>
       <c r="E14" s="19" t="n"/>
       <c r="F14" s="18" t="n"/>
@@ -2742,10 +3635,26 @@
       <c r="K14" s="19" t="n"/>
       <c r="L14" s="18" t="n"/>
       <c r="M14" s="19" t="n"/>
-      <c r="N14" s="16" t="n"/>
-      <c r="O14" s="17" t="n"/>
-      <c r="P14" s="16" t="n"/>
-      <c r="Q14" s="17" t="n"/>
+      <c r="N14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R14" s="18" t="n"/>
       <c r="S14" s="19" t="n"/>
       <c r="T14" s="18" t="n"/>
@@ -2756,10 +3665,26 @@
       <c r="Y14" s="19" t="n"/>
       <c r="Z14" s="18" t="n"/>
       <c r="AA14" s="19" t="n"/>
-      <c r="AB14" s="16" t="n"/>
-      <c r="AC14" s="17" t="n"/>
-      <c r="AD14" s="16" t="n"/>
-      <c r="AE14" s="17" t="n"/>
+      <c r="AB14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF14" s="18" t="n"/>
       <c r="AG14" s="19" t="n"/>
     </row>
@@ -2769,8 +3694,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B15" s="21" t="n"/>
-      <c r="C15" s="22" t="n"/>
+      <c r="B15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D15" s="23" t="n"/>
       <c r="E15" s="24" t="n"/>
       <c r="F15" s="23" t="n"/>
@@ -2781,10 +3714,26 @@
       <c r="K15" s="24" t="n"/>
       <c r="L15" s="23" t="n"/>
       <c r="M15" s="24" t="n"/>
-      <c r="N15" s="21" t="n"/>
-      <c r="O15" s="22" t="n"/>
-      <c r="P15" s="21" t="n"/>
-      <c r="Q15" s="22" t="n"/>
+      <c r="N15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R15" s="23" t="n"/>
       <c r="S15" s="24" t="n"/>
       <c r="T15" s="23" t="n"/>
@@ -2795,10 +3744,26 @@
       <c r="Y15" s="24" t="n"/>
       <c r="Z15" s="23" t="n"/>
       <c r="AA15" s="24" t="n"/>
-      <c r="AB15" s="21" t="n"/>
-      <c r="AC15" s="22" t="n"/>
-      <c r="AD15" s="21" t="n"/>
-      <c r="AE15" s="22" t="n"/>
+      <c r="AB15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF15" s="23" t="n"/>
       <c r="AG15" s="24" t="n"/>
     </row>
@@ -2843,8 +3808,16 @@
           <t>LaSalle</t>
         </is>
       </c>
-      <c r="B17" s="16" t="n"/>
-      <c r="C17" s="17" t="n"/>
+      <c r="B17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D17" s="18" t="n"/>
       <c r="E17" s="19" t="n"/>
       <c r="F17" s="18" t="n"/>
@@ -2855,10 +3828,26 @@
       <c r="K17" s="19" t="n"/>
       <c r="L17" s="18" t="n"/>
       <c r="M17" s="19" t="n"/>
-      <c r="N17" s="16" t="n"/>
-      <c r="O17" s="17" t="n"/>
-      <c r="P17" s="16" t="n"/>
-      <c r="Q17" s="17" t="n"/>
+      <c r="N17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R17" s="18" t="n"/>
       <c r="S17" s="19" t="n"/>
       <c r="T17" s="18" t="n"/>
@@ -2869,10 +3858,26 @@
       <c r="Y17" s="19" t="n"/>
       <c r="Z17" s="18" t="n"/>
       <c r="AA17" s="19" t="n"/>
-      <c r="AB17" s="16" t="n"/>
-      <c r="AC17" s="17" t="n"/>
-      <c r="AD17" s="16" t="n"/>
-      <c r="AE17" s="17" t="n"/>
+      <c r="AB17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF17" s="18" t="n"/>
       <c r="AG17" s="19" t="n"/>
     </row>
@@ -2882,8 +3887,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B18" s="21" t="n"/>
-      <c r="C18" s="22" t="n"/>
+      <c r="B18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D18" s="23" t="n"/>
       <c r="E18" s="24" t="n"/>
       <c r="F18" s="23" t="n"/>
@@ -2894,10 +3907,26 @@
       <c r="K18" s="24" t="n"/>
       <c r="L18" s="23" t="n"/>
       <c r="M18" s="24" t="n"/>
-      <c r="N18" s="21" t="n"/>
-      <c r="O18" s="22" t="n"/>
-      <c r="P18" s="21" t="n"/>
-      <c r="Q18" s="22" t="n"/>
+      <c r="N18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R18" s="23" t="n"/>
       <c r="S18" s="24" t="n"/>
       <c r="T18" s="23" t="n"/>
@@ -2908,10 +3937,26 @@
       <c r="Y18" s="24" t="n"/>
       <c r="Z18" s="23" t="n"/>
       <c r="AA18" s="24" t="n"/>
-      <c r="AB18" s="21" t="n"/>
-      <c r="AC18" s="22" t="n"/>
-      <c r="AD18" s="21" t="n"/>
-      <c r="AE18" s="22" t="n"/>
+      <c r="AB18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF18" s="23" t="n"/>
       <c r="AG18" s="24" t="n"/>
     </row>
@@ -2956,8 +4001,16 @@
           <t>Joliet</t>
         </is>
       </c>
-      <c r="B20" s="16" t="n"/>
-      <c r="C20" s="17" t="n"/>
+      <c r="B20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D20" s="18" t="n"/>
       <c r="E20" s="19" t="n"/>
       <c r="F20" s="18" t="n"/>
@@ -2968,10 +4021,26 @@
       <c r="K20" s="19" t="n"/>
       <c r="L20" s="18" t="n"/>
       <c r="M20" s="19" t="n"/>
-      <c r="N20" s="16" t="n"/>
-      <c r="O20" s="17" t="n"/>
-      <c r="P20" s="16" t="n"/>
-      <c r="Q20" s="17" t="n"/>
+      <c r="N20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R20" s="18" t="n"/>
       <c r="S20" s="19" t="n"/>
       <c r="T20" s="18" t="n"/>
@@ -2982,10 +4051,26 @@
       <c r="Y20" s="19" t="n"/>
       <c r="Z20" s="18" t="n"/>
       <c r="AA20" s="19" t="n"/>
-      <c r="AB20" s="16" t="n"/>
-      <c r="AC20" s="17" t="n"/>
-      <c r="AD20" s="16" t="n"/>
-      <c r="AE20" s="17" t="n"/>
+      <c r="AB20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF20" s="18" t="n"/>
       <c r="AG20" s="19" t="n"/>
     </row>
@@ -2995,8 +4080,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B21" s="21" t="n"/>
-      <c r="C21" s="22" t="n"/>
+      <c r="B21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D21" s="23" t="n"/>
       <c r="E21" s="24" t="n"/>
       <c r="F21" s="23" t="n"/>
@@ -3007,10 +4100,26 @@
       <c r="K21" s="24" t="n"/>
       <c r="L21" s="23" t="n"/>
       <c r="M21" s="24" t="n"/>
-      <c r="N21" s="21" t="n"/>
-      <c r="O21" s="22" t="n"/>
-      <c r="P21" s="21" t="n"/>
-      <c r="Q21" s="22" t="n"/>
+      <c r="N21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R21" s="23" t="n"/>
       <c r="S21" s="24" t="n"/>
       <c r="T21" s="23" t="n"/>
@@ -3021,10 +4130,26 @@
       <c r="Y21" s="24" t="n"/>
       <c r="Z21" s="23" t="n"/>
       <c r="AA21" s="24" t="n"/>
-      <c r="AB21" s="21" t="n"/>
-      <c r="AC21" s="22" t="n"/>
-      <c r="AD21" s="21" t="n"/>
-      <c r="AE21" s="22" t="n"/>
+      <c r="AB21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF21" s="23" t="n"/>
       <c r="AG21" s="24" t="n"/>
     </row>
@@ -3069,8 +4194,16 @@
           <t>Jesse Brown</t>
         </is>
       </c>
-      <c r="B23" s="16" t="n"/>
-      <c r="C23" s="17" t="n"/>
+      <c r="B23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D23" s="18" t="n"/>
       <c r="E23" s="19" t="n"/>
       <c r="F23" s="18" t="n"/>
@@ -3081,10 +4214,26 @@
       <c r="K23" s="19" t="n"/>
       <c r="L23" s="18" t="n"/>
       <c r="M23" s="19" t="n"/>
-      <c r="N23" s="16" t="n"/>
-      <c r="O23" s="17" t="n"/>
-      <c r="P23" s="16" t="n"/>
-      <c r="Q23" s="17" t="n"/>
+      <c r="N23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R23" s="18" t="n"/>
       <c r="S23" s="19" t="n"/>
       <c r="T23" s="18" t="n"/>
@@ -3095,10 +4244,26 @@
       <c r="Y23" s="19" t="n"/>
       <c r="Z23" s="18" t="n"/>
       <c r="AA23" s="19" t="n"/>
-      <c r="AB23" s="16" t="n"/>
-      <c r="AC23" s="17" t="n"/>
-      <c r="AD23" s="16" t="n"/>
-      <c r="AE23" s="17" t="n"/>
+      <c r="AB23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF23" s="18" t="n"/>
       <c r="AG23" s="19" t="n"/>
     </row>
@@ -3108,8 +4273,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B24" s="21" t="n"/>
-      <c r="C24" s="22" t="n"/>
+      <c r="B24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D24" s="23" t="n"/>
       <c r="E24" s="24" t="n"/>
       <c r="F24" s="23" t="n"/>
@@ -3120,10 +4293,26 @@
       <c r="K24" s="24" t="n"/>
       <c r="L24" s="23" t="n"/>
       <c r="M24" s="24" t="n"/>
-      <c r="N24" s="21" t="n"/>
-      <c r="O24" s="22" t="n"/>
-      <c r="P24" s="21" t="n"/>
-      <c r="Q24" s="22" t="n"/>
+      <c r="N24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R24" s="23" t="n"/>
       <c r="S24" s="24" t="n"/>
       <c r="T24" s="23" t="n"/>
@@ -3134,10 +4323,26 @@
       <c r="Y24" s="24" t="n"/>
       <c r="Z24" s="23" t="n"/>
       <c r="AA24" s="24" t="n"/>
-      <c r="AB24" s="21" t="n"/>
-      <c r="AC24" s="22" t="n"/>
-      <c r="AD24" s="21" t="n"/>
-      <c r="AE24" s="22" t="n"/>
+      <c r="AB24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF24" s="23" t="n"/>
       <c r="AG24" s="24" t="n"/>
     </row>
@@ -3182,8 +4387,16 @@
           <t>Crown Point</t>
         </is>
       </c>
-      <c r="B26" s="16" t="n"/>
-      <c r="C26" s="17" t="n"/>
+      <c r="B26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D26" s="18" t="n"/>
       <c r="E26" s="19" t="n"/>
       <c r="F26" s="18" t="n"/>
@@ -3194,10 +4407,26 @@
       <c r="K26" s="19" t="n"/>
       <c r="L26" s="18" t="n"/>
       <c r="M26" s="19" t="n"/>
-      <c r="N26" s="16" t="n"/>
-      <c r="O26" s="17" t="n"/>
-      <c r="P26" s="16" t="n"/>
-      <c r="Q26" s="17" t="n"/>
+      <c r="N26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R26" s="18" t="n"/>
       <c r="S26" s="19" t="n"/>
       <c r="T26" s="18" t="n"/>
@@ -3208,10 +4437,26 @@
       <c r="Y26" s="19" t="n"/>
       <c r="Z26" s="18" t="n"/>
       <c r="AA26" s="19" t="n"/>
-      <c r="AB26" s="16" t="n"/>
-      <c r="AC26" s="17" t="n"/>
-      <c r="AD26" s="16" t="n"/>
-      <c r="AE26" s="17" t="n"/>
+      <c r="AB26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF26" s="18" t="n"/>
       <c r="AG26" s="19" t="n"/>
     </row>
@@ -3221,8 +4466,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B27" s="29" t="n"/>
-      <c r="C27" s="30" t="n"/>
+      <c r="B27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D27" s="31" t="n"/>
       <c r="E27" s="32" t="n"/>
       <c r="F27" s="31" t="n"/>
@@ -3233,10 +4486,26 @@
       <c r="K27" s="32" t="n"/>
       <c r="L27" s="31" t="n"/>
       <c r="M27" s="32" t="n"/>
-      <c r="N27" s="29" t="n"/>
-      <c r="O27" s="30" t="n"/>
-      <c r="P27" s="29" t="n"/>
-      <c r="Q27" s="30" t="n"/>
+      <c r="N27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="R27" s="31" t="n"/>
       <c r="S27" s="32" t="n"/>
       <c r="T27" s="31" t="n"/>
@@ -3247,10 +4516,26 @@
       <c r="Y27" s="32" t="n"/>
       <c r="Z27" s="31" t="n"/>
       <c r="AA27" s="32" t="n"/>
-      <c r="AB27" s="29" t="n"/>
-      <c r="AC27" s="30" t="n"/>
-      <c r="AD27" s="29" t="n"/>
-      <c r="AE27" s="30" t="n"/>
+      <c r="AB27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AD27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AF27" s="31" t="n"/>
       <c r="AG27" s="32" t="n"/>
     </row>

</xml_diff>

<commit_message>
weekends all working, needs holidays and more than 1 month at a time
</commit_message>
<xml_diff>
--- a/cboc_signin_sheet.xlsx
+++ b/cboc_signin_sheet.xlsx
@@ -753,7 +753,7 @@
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: JANUARY 2022</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -2657,7 +2657,7 @@
     <row customHeight="1" ht="45" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Month/Year: MAY 2021</t>
+          <t>Month/Year: JANUARY 2022</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>

</xml_diff>